<commit_message>
Pre snakemake implementation. Haven't PP'd NBr8 yet, could do that with Snakemake too.
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E3BC5FB-92A0-49CF-B44A-3E7D7756A27E}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F1029E6-027C-4EF2-B806-7B4C025219E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -21,12 +21,13 @@
     <sheet name="SFR_limitations" sheetId="9" r:id="rId6"/>
     <sheet name="Categories" sheetId="2" r:id="rId7"/>
     <sheet name="iMOD_bugs" sheetId="10" r:id="rId8"/>
+    <sheet name="RscEst" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NBr!$A$1:$O$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NBr_minor!$A$1:$G$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -558,8 +559,54 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8E0E0613-5620-4CD4-A681-6187F9B32A6D}</author>
+    <author>tc={4C755D57-E80D-4678-A151-E00B776F1F03}</author>
+    <author>tc={93547DE0-9536-496B-8566-6EFCF9FF2A35}</author>
+    <author>tc={7E713826-36E7-4481-BEC8-8BCBDA63C1CC}</author>
+  </authors>
+  <commentList>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{8E0E0613-5620-4CD4-A681-6187F9B32A6D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Just for the .HED file</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{4C755D57-E80D-4678-A151-E00B776F1F03}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Rough estimate, as I'm not sure about all the outputs that'll be produced.</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="2" shapeId="0" xr:uid="{93547DE0-9536-496B-8566-6EFCF9FF2A35}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Assuming 50x speed-up over 1 core.</t>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="3" shapeId="0" xr:uid="{7E713826-36E7-4481-BEC8-8BCBDA63C1CC}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Based on NBr5 (I'm hoping this is an overestimate, as Research cloud should be much faster than OneDrive).
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="265">
   <si>
     <t>#</t>
   </si>
@@ -2030,12 +2077,87 @@
   <si>
     <t>SHD array cannot have nan values, even when the layer thickness is 0 (so those cells become innactive) for some reason.</t>
   </si>
+  <si>
+    <t>Layers</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Cols</t>
+  </si>
+  <si>
+    <t>SPs</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TS (days)</t>
+  </si>
+  <si>
+    <t>B per Val</t>
+  </si>
+  <si>
+    <t>CPU h</t>
+  </si>
+  <si>
+    <t>CPU d</t>
+  </si>
+  <si>
+    <t>CPU SP/h</t>
+  </si>
+  <si>
+    <t>HD Size (GB)</t>
+  </si>
+  <si>
+    <t>Total Size (TB)</t>
+  </si>
+  <si>
+    <t>Sim length (years)</t>
+  </si>
+  <si>
+    <t>Run Dur (60-core)</t>
+  </si>
+  <si>
+    <t>N Brabant 30 year Sim (1 ensemble member)</t>
+  </si>
+  <si>
+    <t>N Brabant 960 year run (all 8 enseble members, 4 emission Scs)</t>
+  </si>
+  <si>
+    <t>Chaamse Beek 30 year Sim (1 enseble member)</t>
+  </si>
+  <si>
+    <t>Chaamse Beek 960 year run (all 8 enseble members, 4 emission Scs)</t>
+  </si>
+  <si>
+    <t>Chaamse Beek Vld run</t>
+  </si>
+  <si>
+    <t>Researc cloud storage cost calcs</t>
+  </si>
+  <si>
+    <t>Duration (days)</t>
+  </si>
+  <si>
+    <t>Cost (credits)</t>
+  </si>
+  <si>
+    <t>Cost/storage/day</t>
+  </si>
+  <si>
+    <t>Storage (TB)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2147,6 +2269,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2600,7 +2729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3111,6 +3240,56 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3279,6 +3458,54 @@
         <a:xfrm>
           <a:off x="628650" y="4410075"/>
           <a:ext cx="7790476" cy="7257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>306456</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE7D1801-8FA5-91BB-6BF6-E1F0BE5CDAA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="46850" b="13173"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2956891"/>
+          <a:ext cx="5599043" cy="5118652"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3773,6 +4000,24 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J1" dT="2025-04-25T10:51:09.87" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{8E0E0613-5620-4CD4-A681-6187F9B32A6D}">
+    <text>Just for the .HED file</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2025-04-25T12:22:08.23" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{4C755D57-E80D-4678-A151-E00B776F1F03}">
+    <text>Rough estimate, as I'm not sure about all the outputs that'll be produced.</text>
+  </threadedComment>
+  <threadedComment ref="O1" dT="2025-04-25T12:40:57.82" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{93547DE0-9536-496B-8566-6EFCF9FF2A35}">
+    <text>Assuming 50x speed-up over 1 core.</text>
+  </threadedComment>
+  <threadedComment ref="L2" dT="2025-04-25T12:29:54.29" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{7E713826-36E7-4481-BEC8-8BCBDA63C1CC}">
+    <text xml:space="preserve">Based on NBr5 (I'm hoping this is an overestimate, as Research cloud should be much faster than OneDrive).
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C4D60B-C912-4DC1-A87D-73F82C7BA5BB}">
   <dimension ref="A1:A3"/>
@@ -3810,12 +4055,12 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E6" sqref="E6"/>
       <selection pane="topRight" activeCell="E6" sqref="E6"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5576,4 +5821,516 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873E6B2-35C4-4A79-9D06-5BB2CD1E5FA3}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="180"/>
+    <col min="12" max="12" width="9.28515625" style="180" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="180"/>
+    <col min="15" max="15" width="9.140625" style="178"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="177" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="175" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="176" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="175" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="J1" s="189" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="190" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" s="183" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" s="184" t="s">
+        <v>248</v>
+      </c>
+      <c r="N1" s="184" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" s="185" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="172">
+        <v>1</v>
+      </c>
+      <c r="D2" s="174">
+        <v>30</v>
+      </c>
+      <c r="E2" s="172">
+        <f>365*D2/C2</f>
+        <v>10950</v>
+      </c>
+      <c r="F2" s="173">
+        <v>37</v>
+      </c>
+      <c r="G2" s="173">
+        <v>344</v>
+      </c>
+      <c r="H2" s="173">
+        <v>480</v>
+      </c>
+      <c r="I2" s="173">
+        <v>4</v>
+      </c>
+      <c r="J2" s="186">
+        <f>ROUND(I2*H2*G2*F2*E2/1024^3,0)</f>
+        <v>249</v>
+      </c>
+      <c r="K2" s="187">
+        <f>J2*4/1024</f>
+        <v>0.97265625</v>
+      </c>
+      <c r="L2" s="179">
+        <f>365*9/36</f>
+        <v>91.25</v>
+      </c>
+      <c r="M2" s="187">
+        <f>E2/L2</f>
+        <v>120</v>
+      </c>
+      <c r="N2" s="191">
+        <f>M2/24</f>
+        <v>5</v>
+      </c>
+      <c r="O2" s="188">
+        <f>N2/50</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="172">
+        <v>1</v>
+      </c>
+      <c r="D3" s="174">
+        <v>960</v>
+      </c>
+      <c r="E3" s="172">
+        <f>365*D3/C3</f>
+        <v>350400</v>
+      </c>
+      <c r="F3" s="173">
+        <v>37</v>
+      </c>
+      <c r="G3" s="173">
+        <v>344</v>
+      </c>
+      <c r="H3" s="173">
+        <v>480</v>
+      </c>
+      <c r="I3" s="173">
+        <v>4</v>
+      </c>
+      <c r="J3" s="186">
+        <f>ROUND(I3*H3*G3*F3*E3/1024^3,0)</f>
+        <v>7975</v>
+      </c>
+      <c r="K3" s="187">
+        <f>J3*4/1024</f>
+        <v>31.15234375</v>
+      </c>
+      <c r="L3" s="179">
+        <f>L2</f>
+        <v>91.25</v>
+      </c>
+      <c r="M3" s="187">
+        <f>E3/L3</f>
+        <v>3840</v>
+      </c>
+      <c r="N3" s="191">
+        <f t="shared" ref="N3:N5" si="0">M3/24</f>
+        <v>160</v>
+      </c>
+      <c r="O3" s="188">
+        <f>N3/50</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="172">
+        <v>1</v>
+      </c>
+      <c r="D4" s="174">
+        <v>30</v>
+      </c>
+      <c r="E4" s="172">
+        <f>E2</f>
+        <v>10950</v>
+      </c>
+      <c r="F4" s="173">
+        <f t="shared" ref="F4:I5" si="1">F2</f>
+        <v>37</v>
+      </c>
+      <c r="G4" s="173">
+        <v>1126</v>
+      </c>
+      <c r="H4" s="173">
+        <v>1503</v>
+      </c>
+      <c r="I4" s="173">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J4" s="186">
+        <f>ROUND(I4*H4*G4*F4*E4/1024^3,0)</f>
+        <v>2554</v>
+      </c>
+      <c r="K4" s="187">
+        <f>J4*4/1024</f>
+        <v>9.9765625</v>
+      </c>
+      <c r="L4" s="179">
+        <f>L2*G2*H2/G4/H4</f>
+        <v>8.902975576378326</v>
+      </c>
+      <c r="M4" s="187">
+        <f>E4/L4</f>
+        <v>1229.9258720930234</v>
+      </c>
+      <c r="N4" s="191">
+        <f t="shared" si="0"/>
+        <v>51.246911337209305</v>
+      </c>
+      <c r="O4" s="188">
+        <f>N4/50</f>
+        <v>1.024938226744186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="172">
+        <v>1</v>
+      </c>
+      <c r="D5" s="174">
+        <v>960</v>
+      </c>
+      <c r="E5" s="172">
+        <f>E3</f>
+        <v>350400</v>
+      </c>
+      <c r="F5" s="173">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="G5" s="173">
+        <v>1126</v>
+      </c>
+      <c r="H5" s="173">
+        <v>1503</v>
+      </c>
+      <c r="I5" s="173">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="186">
+        <f>ROUND(I5*H5*G5*F5*E5/1024^3,0)</f>
+        <v>81738</v>
+      </c>
+      <c r="K5" s="187">
+        <f>J5*4/1024</f>
+        <v>319.2890625</v>
+      </c>
+      <c r="L5" s="179">
+        <f>L3*G3*H3/G5/H5</f>
+        <v>8.902975576378326</v>
+      </c>
+      <c r="M5" s="187">
+        <f>E5/L5</f>
+        <v>39357.627906976748</v>
+      </c>
+      <c r="N5" s="191">
+        <f t="shared" si="0"/>
+        <v>1639.9011627906978</v>
+      </c>
+      <c r="O5" s="188">
+        <f>N5/50</f>
+        <v>32.798023255813952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="172">
+        <v>1</v>
+      </c>
+      <c r="D6" s="174">
+        <v>8</v>
+      </c>
+      <c r="E6" s="172">
+        <f>365*D6/C6</f>
+        <v>2920</v>
+      </c>
+      <c r="F6" s="173">
+        <v>37</v>
+      </c>
+      <c r="G6" s="173">
+        <v>344</v>
+      </c>
+      <c r="H6" s="173">
+        <v>480</v>
+      </c>
+      <c r="I6" s="173">
+        <v>4</v>
+      </c>
+      <c r="J6" s="186">
+        <f>ROUND(I6*H6*G6*F6*E6/1024^3,0)</f>
+        <v>66</v>
+      </c>
+      <c r="K6" s="187">
+        <f>J6*4/1024</f>
+        <v>0.2578125</v>
+      </c>
+      <c r="L6" s="179">
+        <f>365*9/36</f>
+        <v>91.25</v>
+      </c>
+      <c r="M6" s="187">
+        <f>E6/L6</f>
+        <v>32</v>
+      </c>
+      <c r="N6" s="191">
+        <f>M6/24</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O6" s="188">
+        <f>N6/50</f>
+        <v>2.6666666666666665E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="172"/>
+      <c r="D7" s="174"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="173"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="173"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="182"/>
+      <c r="N7" s="192"/>
+      <c r="O7" s="181"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="172"/>
+      <c r="D8" s="174"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="182"/>
+      <c r="L8" s="179"/>
+      <c r="M8" s="182"/>
+      <c r="N8" s="192"/>
+      <c r="O8" s="181"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="172"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="173"/>
+      <c r="H9" s="173"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="182"/>
+      <c r="L9" s="179"/>
+      <c r="M9" s="182"/>
+      <c r="N9" s="192"/>
+      <c r="O9" s="181"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="172"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="179"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="192"/>
+      <c r="O10" s="181"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="172"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="182"/>
+      <c r="L11" s="179"/>
+      <c r="M11" s="182"/>
+      <c r="N11" s="192"/>
+      <c r="O11" s="181"/>
+    </row>
+    <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="194"/>
+      <c r="L13" s="196" t="s">
+        <v>260</v>
+      </c>
+      <c r="M13" s="196"/>
+      <c r="N13" s="196"/>
+      <c r="O13" s="196"/>
+    </row>
+    <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="195"/>
+      <c r="L14" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="M14" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="O14" s="73" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="197">
+        <v>0.99609375</v>
+      </c>
+      <c r="M15" s="180">
+        <v>150</v>
+      </c>
+      <c r="N15" s="180">
+        <v>3473.1</v>
+      </c>
+      <c r="O15" s="178">
+        <f>N15/M15/L15</f>
+        <v>23.244800000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L16" s="197">
+        <v>0.4931640625</v>
+      </c>
+      <c r="M16" s="180">
+        <v>150</v>
+      </c>
+      <c r="N16" s="180">
+        <v>1719.5</v>
+      </c>
+      <c r="O16" s="178">
+        <f t="shared" ref="O16:O17" si="2">N16/M16/L16</f>
+        <v>23.244462046204621</v>
+      </c>
+    </row>
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L17" s="197">
+        <v>0.4931640625</v>
+      </c>
+      <c r="M17" s="180">
+        <v>300</v>
+      </c>
+      <c r="N17" s="180">
+        <v>3439.1</v>
+      </c>
+      <c r="O17" s="178">
+        <f t="shared" si="2"/>
+        <v>23.245137953795378</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L13:O13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NBr11 improvements, NBr12 run, WS_Mdl improvements.
NBr11: Smk improvements (DT logging) + re-run to test. NBr12: run via Smk, still not PoPed. Added Sim_Cfg terminal function. WS_Mdl: minor bug, cosmetics, Smk addition to S_from_B, lock addition to Up_log (to avoid corrupted files), permission now required to reset_Sim.
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="541" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F1029E6-027C-4EF2-B806-7B4C025219E7}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4E2FD58-CE8A-4289-A739-7DF2CF901B7C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,6 +566,7 @@
     <author>tc={4C755D57-E80D-4678-A151-E00B776F1F03}</author>
     <author>tc={93547DE0-9536-496B-8566-6EFCF9FF2A35}</author>
     <author>tc={7E713826-36E7-4481-BEC8-8BCBDA63C1CC}</author>
+    <author>tc={F1BEC491-BB3D-421D-B1D1-B5EC7D86B0DA}</author>
   </authors>
   <commentList>
     <comment ref="J1" authorId="0" shapeId="0" xr:uid="{8E0E0613-5620-4CD4-A681-6187F9B32A6D}">
@@ -601,12 +602,20 @@
 </t>
       </text>
     </comment>
+    <comment ref="J14" authorId="4" shapeId="0" xr:uid="{F1BEC491-BB3D-421D-B1D1-B5EC7D86B0DA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Just for the .HED file</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="266">
   <si>
     <t>#</t>
   </si>
@@ -2148,6 +2157,9 @@
   </si>
   <si>
     <t>Storage (TB)</t>
+  </si>
+  <si>
+    <t>HD size calc</t>
   </si>
 </sst>
 </file>
@@ -2157,7 +2169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2276,6 +2288,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2729,7 +2747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3286,10 +3304,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3504,7 +3525,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2956891"/>
+          <a:off x="0" y="3155674"/>
           <a:ext cx="5599043" cy="5118652"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4015,6 +4036,9 @@
     <text xml:space="preserve">Based on NBr5 (I'm hoping this is an overestimate, as Research cloud should be much faster than OneDrive).
 </text>
   </threadedComment>
+  <threadedComment ref="J14" dT="2025-04-25T10:51:09.87" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{F1BEC491-BB3D-421D-B1D1-B5EC7D86B0DA}">
+    <text>Just for the .HED file</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -5831,7 +5855,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6257,15 +6281,41 @@
       <c r="O11" s="181"/>
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="198" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13" s="198"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="198"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="198"/>
       <c r="K13" s="194"/>
-      <c r="L13" s="196" t="s">
+      <c r="L13" s="197" t="s">
         <v>260</v>
       </c>
-      <c r="M13" s="196"/>
-      <c r="N13" s="196"/>
-      <c r="O13" s="196"/>
+      <c r="M13" s="197"/>
+      <c r="N13" s="197"/>
+      <c r="O13" s="197"/>
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="175" t="s">
+        <v>244</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="H14" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="I14" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="J14" s="189" t="s">
+        <v>251</v>
+      </c>
       <c r="K14" s="195"/>
       <c r="L14" s="73" t="s">
         <v>264</v>
@@ -6281,7 +6331,30 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L15" s="197">
+      <c r="E15">
+        <f>9*265</f>
+        <v>2385</v>
+      </c>
+      <c r="F15">
+        <f>F2</f>
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <f>G2</f>
+        <v>344</v>
+      </c>
+      <c r="H15">
+        <f>H2</f>
+        <v>480</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15" s="186">
+        <f>ROUND(I15*H15*G15*F15*E15/1024^3,0)</f>
+        <v>109</v>
+      </c>
+      <c r="L15" s="196">
         <v>0.99609375</v>
       </c>
       <c r="M15" s="180">
@@ -6296,7 +6369,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L16" s="197">
+      <c r="L16" s="196">
         <v>0.4931640625</v>
       </c>
       <c r="M16" s="180">
@@ -6311,7 +6384,7 @@
       </c>
     </row>
     <row r="17" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L17" s="197">
+      <c r="L17" s="196">
         <v>0.4931640625</v>
       </c>
       <c r="M17" s="180">
@@ -6326,8 +6399,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L13:O13"/>
+    <mergeCell ref="E13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Minor hanges before I fix DVC double-storage
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4E2FD58-CE8A-4289-A739-7DF2CF901B7C}"/>
+  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1C813E-B1D9-4AAC-ACC6-E4FAD3A7B589}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NBr!$A$1:$O$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NBr_minor!$A$1:$G$14</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="266">
   <si>
     <t>#</t>
   </si>
@@ -2169,7 +2169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2288,12 +2288,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -5855,7 +5849,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6332,8 +6326,8 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E15">
-        <f>9*265</f>
-        <v>2385</v>
+        <f>9*365</f>
+        <v>3285</v>
       </c>
       <c r="F15">
         <f>F2</f>
@@ -6351,8 +6345,8 @@
         <v>8</v>
       </c>
       <c r="J15" s="186">
-        <f>ROUND(I15*H15*G15*F15*E15/1024^3,0)</f>
-        <v>109</v>
+        <f>ROUND(I15*H15*G15*F15*E15/1024^3,1)</f>
+        <v>149.5</v>
       </c>
       <c r="L15" s="196">
         <v>0.99609375</v>

</xml_diff>

<commit_message>
Ran NBr16. Improved env management. NBr13 PoP workflow setup not finished yet.
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1C813E-B1D9-4AAC-ACC6-E4FAD3A7B589}"/>
+  <xr:revisionPtr revIDLastSave="571" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{242DE3BF-A0E4-4D32-B38C-4A56A597FA2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294966606" uniqueCount="266">
   <si>
     <t>#</t>
   </si>
@@ -1112,52 +1112,10 @@
     <t>Week of end</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Creation of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Roboto"/>
-      </rPr>
-      <t>SimLog</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Roboto"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Roboto"/>
-      </rPr>
-      <t xml:space="preserve">SimMng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Roboto"/>
-      </rPr>
-      <t>code</t>
-    </r>
-  </si>
-  <si>
     <t>Final Decision For/Against Improvement</t>
   </si>
   <si>
     <t>IMO it's essential to record and document Sims in a clean and organised manner, to avoid future confusion and potential mistakes. For that reason I'll make a spreadsheet catalog for all our Sims and a governing script that will run the model based on the spreadsheet.</t>
-  </si>
-  <si>
-    <t>This works in combination with the use of Sim numbers. It's an overall system for keeping track of changes.</t>
   </si>
   <si>
     <t>Implementation Steps</t>
@@ -2160,6 +2118,48 @@
   </si>
   <si>
     <t>HD size calc</t>
+  </si>
+  <si>
+    <t>This works in combination with the use of MdlNs. It's an overall system for keeping track of changes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creation of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>RunLog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve">RunMng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>code</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2741,7 +2741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3304,6 +3304,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4048,17 +4051,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4071,14 +4074,14 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E6" sqref="E6"/>
       <selection pane="topRight" activeCell="E6" sqref="E6"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4096,10 +4099,13 @@
     <col min="13" max="14" width="8.7109375" style="92" customWidth="1"/>
     <col min="15" max="15" width="60.7109375" style="67" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" style="67" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="24"/>
+    <col min="17" max="19" width="9.140625" style="24"/>
+    <col min="20" max="20" width="12.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="22" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="22" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>54</v>
       </c>
       <c r="H1" s="70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I1" s="70" t="s">
         <v>88</v>
@@ -4146,12 +4152,12 @@
         <v>8</v>
       </c>
       <c r="P1" s="68" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="121" customFormat="1" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="121" customFormat="1" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>111</v>
+        <v>265</v>
       </c>
       <c r="B2" s="109" t="s">
         <v>87</v>
@@ -4175,7 +4181,7 @@
         <v>98</v>
       </c>
       <c r="I2" s="116" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J2" s="117">
         <v>10</v>
@@ -4193,11 +4199,11 @@
         <v>3</v>
       </c>
       <c r="O2" s="120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P2" s="120"/>
     </row>
-    <row r="3" spans="1:16" s="128" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="128" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
@@ -4223,7 +4229,7 @@
         <v>98</v>
       </c>
       <c r="I3" s="123" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J3" s="124">
         <v>10</v>
@@ -4243,13 +4249,13 @@
         <v>3</v>
       </c>
       <c r="O3" s="127" t="s">
+        <v>264</v>
+      </c>
+      <c r="P3" s="127"/>
+    </row>
+    <row r="4" spans="1:20" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="93" t="s">
         <v>114</v>
-      </c>
-      <c r="P3" s="127"/>
-    </row>
-    <row r="4" spans="1:16" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
-        <v>116</v>
       </c>
       <c r="B4" s="94" t="s">
         <v>87</v>
@@ -4258,22 +4264,22 @@
         <v>75</v>
       </c>
       <c r="D4" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="97" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="98" t="s">
-        <v>119</v>
-      </c>
       <c r="G4" s="99" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H4" s="100" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I4" s="101" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J4" s="102">
         <v>10</v>
@@ -4293,11 +4299,11 @@
         <v>3</v>
       </c>
       <c r="O4" s="106" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P4" s="106"/>
     </row>
-    <row r="5" spans="1:16" s="143" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="143" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="129" t="s">
         <v>90</v>
       </c>
@@ -4323,7 +4329,7 @@
         <v>74</v>
       </c>
       <c r="I5" s="137" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J5" s="138">
         <v>9</v>
@@ -4347,7 +4353,7 @@
       </c>
       <c r="P5" s="142"/>
     </row>
-    <row r="6" spans="1:16" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="146" t="s">
         <v>38</v>
       </c>
@@ -4373,7 +4379,7 @@
         <v>99</v>
       </c>
       <c r="I6" s="101" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J6" s="102">
         <v>8</v>
@@ -4397,7 +4403,7 @@
       </c>
       <c r="P6" s="106"/>
     </row>
-    <row r="7" spans="1:16" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="93" t="s">
         <v>91</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>101</v>
       </c>
       <c r="I7" s="155" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J7" s="102">
         <v>7</v>
@@ -4447,7 +4453,7 @@
       </c>
       <c r="P7" s="106"/>
     </row>
-    <row r="8" spans="1:16" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="93" t="s">
         <v>92</v>
       </c>
@@ -4473,7 +4479,7 @@
         <v>104</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J8" s="102">
         <v>6</v>
@@ -4497,7 +4503,7 @@
       </c>
       <c r="P8" s="106"/>
     </row>
-    <row r="9" spans="1:16" s="25" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="25" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>93</v>
       </c>
@@ -4523,7 +4529,7 @@
         <v>103</v>
       </c>
       <c r="I9" s="84" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J9" s="59">
         <v>5</v>
@@ -4546,8 +4552,9 @@
         <v>37</v>
       </c>
       <c r="P9" s="47"/>
-    </row>
-    <row r="10" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T9" s="199"/>
+    </row>
+    <row r="10" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>95</v>
       </c>
@@ -4573,7 +4580,7 @@
         <v>107</v>
       </c>
       <c r="I10" s="84" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J10" s="59">
         <v>5</v>
@@ -4597,33 +4604,33 @@
       </c>
       <c r="P10" s="47"/>
     </row>
-    <row r="11" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="79" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" s="79" t="s">
-        <v>148</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="81" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="E11" s="82" t="s">
+      <c r="F11" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="H11" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="83" t="s">
-        <v>151</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>152</v>
-      </c>
       <c r="I11" s="84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J11" s="59">
         <v>5</v>
@@ -4643,11 +4650,11 @@
         <v>16</v>
       </c>
       <c r="O11" s="47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P11" s="47"/>
     </row>
-    <row r="12" spans="1:16" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="107" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="93" t="s">
         <v>97</v>
       </c>
@@ -4670,10 +4677,10 @@
         <v>67</v>
       </c>
       <c r="H12" s="165" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I12" s="166" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J12" s="167">
         <v>4</v>
@@ -4697,7 +4704,7 @@
       </c>
       <c r="P12" s="171"/>
     </row>
-    <row r="13" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>94</v>
       </c>
@@ -4723,7 +4730,7 @@
         <v>106</v>
       </c>
       <c r="I13" s="84" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J13" s="45">
         <v>3</v>
@@ -4747,9 +4754,9 @@
       </c>
       <c r="P13" s="47"/>
     </row>
-    <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="79" t="s">
         <v>5</v>
@@ -4770,10 +4777,10 @@
         <v>80</v>
       </c>
       <c r="H14" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I14" s="84" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J14" s="45">
         <v>2</v>
@@ -4797,7 +4804,7 @@
       </c>
       <c r="P14" s="47"/>
     </row>
-    <row r="15" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>96</v>
       </c>
@@ -4820,10 +4827,10 @@
         <v>69</v>
       </c>
       <c r="H15" s="43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I15" s="84" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J15" s="45">
         <v>1</v>
@@ -4884,27 +4891,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="144" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="144">
         <v>1</v>
@@ -4912,10 +4919,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="144" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="144">
         <v>1</v>
@@ -4923,10 +4930,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="144" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" s="144">
         <v>1</v>
@@ -4934,10 +4941,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="144" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E5" s="144">
         <v>1</v>
@@ -4945,10 +4952,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="144" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D6" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E6" s="144">
         <v>1</v>
@@ -4956,10 +4963,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="144" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="144">
         <v>1</v>
@@ -4967,10 +4974,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="144" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D8" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E8" s="144">
         <v>1</v>
@@ -4978,10 +4985,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="144" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D9" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" s="144">
         <v>1</v>
@@ -4989,10 +4996,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="144" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D10" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E10" s="144">
         <v>1</v>
@@ -5000,10 +5007,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="144" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D11" s="144" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" s="144">
         <v>1</v>
@@ -5011,13 +5018,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="144" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D12" s="144" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="144">
         <v>1</v>
@@ -5028,18 +5035,18 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="144" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D13" s="144" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="144" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D14" s="144" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5072,48 +5079,48 @@
   <sheetData>
     <row r="1" spans="1:12" s="74" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="73" t="s">
+      <c r="D1" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="E1" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="J1" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="77" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>201</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="75" t="s">
-        <v>139</v>
-      </c>
       <c r="L1" s="75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
         <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
       </c>
       <c r="D2" s="76">
         <v>29221</v>
@@ -5122,21 +5129,21 @@
         <v>44109</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D3" s="76">
         <v>29221</v>
@@ -5145,24 +5152,24 @@
         <v>44109</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4">
         <v>4749</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" s="76">
         <v>39083</v>
@@ -5171,21 +5178,21 @@
         <v>43831</v>
       </c>
       <c r="G4" s="76" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D5" s="76">
         <v>27760</v>
@@ -5197,27 +5204,27 @@
         <v>46023</v>
       </c>
       <c r="G5" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="H5" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L5" t="s">
         <v>205</v>
-      </c>
-      <c r="H5" s="76" t="s">
-        <v>143</v>
-      </c>
-      <c r="J5" t="s">
-        <v>206</v>
-      </c>
-      <c r="L5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B6">
         <v>860</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="76">
         <v>34335</v>
@@ -5229,27 +5236,27 @@
         <v>45658</v>
       </c>
       <c r="G6" s="76" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H6" s="76" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B7">
         <v>826</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D7" s="76">
         <v>27760</v>
@@ -5261,24 +5268,24 @@
         <v>46023</v>
       </c>
       <c r="G7" s="76" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B8">
         <v>11656</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D8" s="76">
         <v>33970</v>
@@ -5287,10 +5294,10 @@
         <v>43462</v>
       </c>
       <c r="G8" s="76" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H8" s="76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5343,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>4</v>
@@ -5355,21 +5362,21 @@
         <v>39</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G1" s="70" t="s">
         <v>88</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32">
@@ -5384,17 +5391,17 @@
     </row>
     <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="39">
         <v>8</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="37"/>
@@ -5402,17 +5409,17 @@
     </row>
     <row r="4" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C4" s="45"/>
       <c r="D4" s="46">
         <v>8</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="44"/>
@@ -5420,7 +5427,7 @@
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B5" s="53"/>
       <c r="C5" s="51"/>
@@ -5432,10 +5439,10 @@
     </row>
     <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C6" s="45"/>
       <c r="D6" s="46"/>
@@ -5446,10 +5453,10 @@
     </row>
     <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="58"/>
@@ -5559,13 +5566,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="150" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C1" s="150" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D1" s="150" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5573,13 +5580,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="152" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C2" s="152" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D2" s="152" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -5587,13 +5594,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="152" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C3" s="152" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D3" s="152" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5601,13 +5608,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="152" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D4" s="152" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5615,13 +5622,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="152" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C5" s="152" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D5" s="152" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5629,13 +5636,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="152" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C6" s="152" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D6" s="152" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5643,7 +5650,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="152" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5824,7 +5831,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5832,7 +5839,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5848,7 +5855,7 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -5868,46 +5875,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="175" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="176" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="175" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="73" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="J1" s="189" t="s">
+        <v>249</v>
+      </c>
+      <c r="K1" s="190" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1" s="183" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" s="184" t="s">
         <v>246</v>
       </c>
-      <c r="D1" s="176" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" s="175" t="s">
-        <v>244</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="73" t="s">
+      <c r="N1" s="184" t="s">
         <v>247</v>
       </c>
-      <c r="J1" s="189" t="s">
-        <v>251</v>
-      </c>
-      <c r="K1" s="190" t="s">
+      <c r="O1" s="185" t="s">
         <v>252</v>
-      </c>
-      <c r="L1" s="183" t="s">
-        <v>250</v>
-      </c>
-      <c r="M1" s="184" t="s">
-        <v>248</v>
-      </c>
-      <c r="N1" s="184" t="s">
-        <v>249</v>
-      </c>
-      <c r="O1" s="185" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5915,7 +5922,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C2" s="172">
         <v>1</v>
@@ -5969,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C3" s="172">
         <v>1</v>
@@ -6023,7 +6030,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C4" s="172">
         <v>1</v>
@@ -6079,7 +6086,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C5" s="172">
         <v>1</v>
@@ -6135,7 +6142,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C6" s="172">
         <v>1</v>
@@ -6276,7 +6283,7 @@
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E13" s="198" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F13" s="198"/>
       <c r="G13" s="198"/>
@@ -6285,7 +6292,7 @@
       <c r="J13" s="198"/>
       <c r="K13" s="194"/>
       <c r="L13" s="197" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M13" s="197"/>
       <c r="N13" s="197"/>
@@ -6293,35 +6300,35 @@
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F14" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="H14" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="G14" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="H14" s="73" t="s">
-        <v>243</v>
-      </c>
       <c r="I14" s="73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="73" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M14" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="O14" s="73" t="s">
         <v>261</v>
-      </c>
-      <c r="N14" s="73" t="s">
-        <v>262</v>
-      </c>
-      <c r="O14" s="73" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Quicker paths. Efficient Mdl file openning
get_MdlN_Pa: was created. It's a better version of get_MdlN_paths.
open_:was created. Helps with opening common model files quickly and efficiently.
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="998" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E73E1CF4-727C-46E4-9A7D-5855A7D8CF5A}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4025F9E-5B43-4127-99E0-446DEFFF582C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
     <sheet name="NBr" sheetId="1" r:id="rId2"/>
-    <sheet name="SFR_requirements" sheetId="8" r:id="rId3"/>
+    <sheet name="SFR_requirements" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="NBr_TS_Ext" sheetId="7" r:id="rId4"/>
     <sheet name="NBr_minor" sheetId="6" r:id="rId5"/>
     <sheet name="SFR_limitations" sheetId="9" r:id="rId6"/>
     <sheet name="Categories" sheetId="2" r:id="rId7"/>
     <sheet name="iMOD_bugs" sheetId="10" r:id="rId8"/>
     <sheet name="RscEst" sheetId="11" r:id="rId9"/>
-    <sheet name="Shp_eval" sheetId="14" r:id="rId10"/>
+    <sheet name="SFR_Shp_eval" sheetId="14" r:id="rId10"/>
     <sheet name="SFR_extra_system_error" sheetId="12" state="hidden" r:id="rId11"/>
     <sheet name="SFR_extra_system_error (2)" sheetId="13" state="hidden" r:id="rId12"/>
   </sheets>
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294967004" uniqueCount="310">
   <si>
     <t>#</t>
   </si>
@@ -2333,7 +2333,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2473,12 +2473,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3773,45 +3767,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
@@ -3823,6 +3778,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4607,7 +4601,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4624,21 +4618,21 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="257" t="s">
+      <c r="A3" s="244" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="258" t="s">
+      <c r="B3" s="245" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="258" t="s">
+      <c r="C3" s="245" t="s">
         <v>299</v>
       </c>
-      <c r="D3" s="259" t="s">
+      <c r="D3" s="246" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="252">
+      <c r="A4" s="239">
         <v>1</v>
       </c>
       <c r="B4" s="173" t="s">
@@ -4647,10 +4641,10 @@
       <c r="C4" s="173" t="s">
         <v>300</v>
       </c>
-      <c r="D4" s="253"/>
+      <c r="D4" s="240"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="252">
+      <c r="A5" s="239">
         <v>2</v>
       </c>
       <c r="B5" s="173" t="s">
@@ -4659,10 +4653,10 @@
       <c r="C5" s="173" t="s">
         <v>300</v>
       </c>
-      <c r="D5" s="253"/>
+      <c r="D5" s="240"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="252">
+      <c r="A6" s="239">
         <v>3</v>
       </c>
       <c r="B6" s="173" t="s">
@@ -4671,10 +4665,10 @@
       <c r="C6" s="173" t="s">
         <v>300</v>
       </c>
-      <c r="D6" s="253"/>
+      <c r="D6" s="240"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="252">
+      <c r="A7" s="239">
         <v>4</v>
       </c>
       <c r="B7" s="173" t="s">
@@ -4683,10 +4677,10 @@
       <c r="C7" s="173" t="s">
         <v>300</v>
       </c>
-      <c r="D7" s="253"/>
+      <c r="D7" s="240"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="252">
+      <c r="A8" s="239">
         <v>5</v>
       </c>
       <c r="B8" s="173" t="s">
@@ -4695,129 +4689,129 @@
       <c r="C8" s="173" t="s">
         <v>301</v>
       </c>
-      <c r="D8" s="253" t="s">
+      <c r="D8" s="240" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="252">
+      <c r="A9" s="239">
         <v>6</v>
       </c>
       <c r="B9" s="173" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="260" t="s">
+      <c r="C9" s="247" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="253" t="s">
+      <c r="D9" s="240" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="252">
+      <c r="A10" s="239">
         <v>7</v>
       </c>
       <c r="B10" s="173" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="260" t="s">
+      <c r="C10" s="247" t="s">
         <v>301</v>
       </c>
-      <c r="D10" s="253" t="s">
+      <c r="D10" s="240" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="252">
+      <c r="A11" s="239">
         <v>8</v>
       </c>
       <c r="B11" s="173" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="260" t="s">
+      <c r="C11" s="247" t="s">
         <v>301</v>
       </c>
-      <c r="D11" s="253" t="s">
+      <c r="D11" s="240" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="252">
+      <c r="A12" s="239">
         <v>9</v>
       </c>
       <c r="B12" s="173" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="260" t="s">
+      <c r="C12" s="247" t="s">
         <v>306</v>
       </c>
-      <c r="D12" s="253" t="s">
+      <c r="D12" s="240" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="252">
+      <c r="A13" s="239">
         <v>10</v>
       </c>
       <c r="B13" s="173" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="260" t="s">
+      <c r="C13" s="247" t="s">
         <v>306</v>
       </c>
-      <c r="D13" s="253" t="s">
+      <c r="D13" s="240" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="252">
+      <c r="A14" s="239">
         <v>11</v>
       </c>
       <c r="B14" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="260" t="s">
+      <c r="C14" s="247" t="s">
         <v>306</v>
       </c>
-      <c r="D14" s="253" t="s">
+      <c r="D14" s="240" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="252">
+      <c r="A15" s="239">
         <v>12</v>
       </c>
       <c r="B15" s="173" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="260" t="s">
+      <c r="C15" s="247" t="s">
         <v>300</v>
       </c>
-      <c r="D15" s="253"/>
+      <c r="D15" s="240"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="252">
+      <c r="A16" s="239">
         <v>13</v>
       </c>
       <c r="B16" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="260" t="s">
+      <c r="C16" s="247" t="s">
         <v>300</v>
       </c>
-      <c r="D16" s="253"/>
+      <c r="D16" s="240"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="254">
+      <c r="A17" s="241">
         <v>14</v>
       </c>
-      <c r="B17" s="255" t="s">
+      <c r="B17" s="242" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="261" t="s">
+      <c r="C17" s="248" t="s">
         <v>300</v>
       </c>
-      <c r="D17" s="256"/>
+      <c r="D17" s="243"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4891,50 +4885,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="246" t="s">
+      <c r="B6" s="257" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="247"/>
-      <c r="D6" s="247"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="258"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="248" t="s">
+      <c r="F6" s="259" t="s">
         <v>287</v>
       </c>
-      <c r="G6" s="248"/>
-      <c r="H6" s="248"/>
-      <c r="I6" s="248"/>
-      <c r="J6" s="248"/>
+      <c r="G6" s="259"/>
+      <c r="H6" s="259"/>
+      <c r="I6" s="259"/>
+      <c r="J6" s="259"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="244" t="s">
+      <c r="B7" s="255" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
+      <c r="C7" s="256"/>
+      <c r="D7" s="256"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="243" t="s">
+      <c r="F7" s="254" t="s">
         <v>274</v>
       </c>
-      <c r="G7" s="243"/>
-      <c r="H7" s="243"/>
-      <c r="I7" s="243"/>
-      <c r="J7" s="243"/>
+      <c r="G7" s="254"/>
+      <c r="H7" s="254"/>
+      <c r="I7" s="254"/>
+      <c r="J7" s="254"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="240" t="s">
+      <c r="B8" s="251" t="s">
         <v>290</v>
       </c>
-      <c r="C8" s="241"/>
+      <c r="C8" s="252"/>
       <c r="D8" s="225" t="s">
         <v>277</v>
       </c>
       <c r="E8" s="210"/>
-      <c r="F8" s="242" t="s">
+      <c r="F8" s="253" t="s">
         <v>290</v>
       </c>
-      <c r="G8" s="242"/>
+      <c r="G8" s="253"/>
       <c r="H8" s="232" t="s">
         <v>277</v>
       </c>
@@ -5579,7 +5573,7 @@
       <c r="J34" s="219"/>
     </row>
     <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="251" t="s">
+      <c r="A35" s="238" t="s">
         <v>293</v>
       </c>
       <c r="B35" s="200"/>
@@ -6249,50 +6243,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="246" t="s">
+      <c r="B6" s="257" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="247"/>
-      <c r="D6" s="247"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="258"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="248" t="s">
+      <c r="F6" s="259" t="s">
         <v>287</v>
       </c>
-      <c r="G6" s="248"/>
-      <c r="H6" s="248"/>
-      <c r="I6" s="248"/>
-      <c r="J6" s="248"/>
+      <c r="G6" s="259"/>
+      <c r="H6" s="259"/>
+      <c r="I6" s="259"/>
+      <c r="J6" s="259"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="244" t="s">
+      <c r="B7" s="255" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
+      <c r="C7" s="256"/>
+      <c r="D7" s="256"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="243" t="s">
+      <c r="F7" s="254" t="s">
         <v>274</v>
       </c>
-      <c r="G7" s="243"/>
-      <c r="H7" s="243"/>
-      <c r="I7" s="243"/>
-      <c r="J7" s="243"/>
+      <c r="G7" s="254"/>
+      <c r="H7" s="254"/>
+      <c r="I7" s="254"/>
+      <c r="J7" s="254"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="249" t="s">
+      <c r="B8" s="260" t="s">
         <v>290</v>
       </c>
-      <c r="C8" s="250"/>
+      <c r="C8" s="261"/>
       <c r="D8" s="236" t="s">
         <v>277</v>
       </c>
       <c r="E8" s="209"/>
-      <c r="F8" s="242" t="s">
+      <c r="F8" s="253" t="s">
         <v>290</v>
       </c>
-      <c r="G8" s="242"/>
+      <c r="G8" s="253"/>
       <c r="H8" s="232" t="s">
         <v>277</v>
       </c>
@@ -10339,21 +10333,21 @@
       <c r="O11" s="181"/>
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="239" t="s">
+      <c r="E13" s="250" t="s">
         <v>263</v>
       </c>
-      <c r="F13" s="239"/>
-      <c r="G13" s="239"/>
-      <c r="H13" s="239"/>
-      <c r="I13" s="239"/>
-      <c r="J13" s="239"/>
+      <c r="F13" s="250"/>
+      <c r="G13" s="250"/>
+      <c r="H13" s="250"/>
+      <c r="I13" s="250"/>
+      <c r="J13" s="250"/>
       <c r="K13" s="194"/>
-      <c r="L13" s="238" t="s">
+      <c r="L13" s="249" t="s">
         <v>258</v>
       </c>
-      <c r="M13" s="238"/>
-      <c r="N13" s="238"/>
-      <c r="O13" s="238"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">

</xml_diff>

<commit_message>
NBr29 attempt (i.e. MVR:DRN->SFR)
NBr29 attempt
gitignored .lnk (shortcuts)
QGIS/Sblg/NS: added min and max options
utils: added MF6_block_to_DF add_MVR_to options
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1000" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4025F9E-5B43-4127-99E0-446DEFFF582C}"/>
+  <xr:revisionPtr revIDLastSave="1007" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78ED0F2A-009B-49A0-9711-02D9C8305B74}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="SFR_requirements" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="NBr_TS_Ext" sheetId="7" r:id="rId4"/>
     <sheet name="NBr_minor" sheetId="6" r:id="rId5"/>
-    <sheet name="SFR_limitations" sheetId="9" r:id="rId6"/>
-    <sheet name="Categories" sheetId="2" r:id="rId7"/>
-    <sheet name="iMOD_bugs" sheetId="10" r:id="rId8"/>
-    <sheet name="RscEst" sheetId="11" r:id="rId9"/>
-    <sheet name="SFR_Shp_eval" sheetId="14" r:id="rId10"/>
+    <sheet name="Categories" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="SFR_limitations" sheetId="9" r:id="rId7"/>
+    <sheet name="SFR_Shp_eval" sheetId="14" r:id="rId8"/>
+    <sheet name="iMOD_bugs" sheetId="10" r:id="rId9"/>
+    <sheet name="RscEst" sheetId="11" r:id="rId10"/>
     <sheet name="SFR_extra_system_error" sheetId="12" state="hidden" r:id="rId11"/>
     <sheet name="SFR_extra_system_error (2)" sheetId="13" state="hidden" r:id="rId12"/>
   </sheets>
@@ -565,6 +565,34 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}</author>
+    <author>tc={92B32FC7-1C92-4272-8FCD-D336DE04F42E}</author>
+  </authors>
+  <commentList>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    There is a problem: bodemhoogste is available on website, length comes from shapefiles.
+We could match the cross sections to the 1ry/2ry/3ry shapefiles though.</t>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="1" shapeId="0" xr:uid="{92B32FC7-1C92-4272-8FCD-D336DE04F42E}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    SFR - RS vs Datasets for SFR </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={8E0E0613-5620-4CD4-A681-6187F9B32A6D}</author>
     <author>tc={4C755D57-E80D-4678-A151-E00B776F1F03}</author>
     <author>tc={93547DE0-9536-496B-8566-6EFCF9FF2A35}</author>
@@ -617,36 +645,8 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}</author>
-    <author>tc={92B32FC7-1C92-4272-8FCD-D336DE04F42E}</author>
-  </authors>
-  <commentList>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    There is a problem: bodemhoogste is available on website, length comes from shapefiles.
-We could match the cross sections to the 1ry/2ry/3ry shapefiles though.</t>
-      </text>
-    </comment>
-    <comment ref="D12" authorId="1" shapeId="0" xr:uid="{92B32FC7-1C92-4272-8FCD-D336DE04F42E}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    SFR - RS vs Datasets for SFR </t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294967004" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="310">
   <si>
     <t>#</t>
   </si>
@@ -4529,6 +4529,24 @@
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D10" dT="2025-07-04T11:54:06.61" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}">
+    <text>There is a problem: bodemhoogste is available on website, length comes from shapefiles.
+We could match the cross sections to the 1ry/2ry/3ry shapefiles though.</text>
+  </threadedComment>
+  <threadedComment ref="D12" dT="2025-07-04T12:02:21.53" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{92B32FC7-1C92-4272-8FCD-D336DE04F42E}">
+    <text xml:space="preserve">SFR - RS vs Datasets for SFR </text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3686889673</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="28" url="https://chatgpt.com/c/6867a333-b440-8010-8270-fea663d00a8b"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="J1" dT="2025-04-25T10:51:09.87" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{8E0E0613-5620-4CD4-A681-6187F9B32A6D}">
     <text>Just for the .HED file</text>
   </threadedComment>
@@ -4548,24 +4566,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D10" dT="2025-07-04T11:54:06.61" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{D4793487-D6C1-476E-A8B2-FA7E49FEE0CB}">
-    <text>There is a problem: bodemhoogste is available on website, length comes from shapefiles.
-We could match the cross sections to the 1ry/2ry/3ry shapefiles though.</text>
-  </threadedComment>
-  <threadedComment ref="D12" dT="2025-07-04T12:02:21.53" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{92B32FC7-1C92-4272-8FCD-D336DE04F42E}">
-    <text xml:space="preserve">SFR - RS vs Datasets for SFR </text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>3686889673</xltc2:checksum>
-        <xltc2:hyperlink startIndex="0" length="28" url="https://chatgpt.com/c/6867a333-b440-8010-8270-fea663d00a8b"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C4D60B-C912-4DC1-A87D-73F82C7BA5BB}">
   <dimension ref="A1:A3"/>
@@ -4597,225 +4597,564 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9E9723-48CB-44D6-9690-AF1878CFBFAF}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873E6B2-35C4-4A79-9D06-5BB2CD1E5FA3}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="159.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="180"/>
+    <col min="12" max="12" width="9.28515625" style="180" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="180"/>
+    <col min="15" max="15" width="9.140625" style="178"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="244" t="s">
+    <row r="1" spans="1:15" s="177" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="245" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="245" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="246" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="239">
+      <c r="B1" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="175" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="176" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="175" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>245</v>
+      </c>
+      <c r="J1" s="189" t="s">
+        <v>249</v>
+      </c>
+      <c r="K1" s="190" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1" s="183" t="s">
+        <v>248</v>
+      </c>
+      <c r="M1" s="184" t="s">
+        <v>246</v>
+      </c>
+      <c r="N1" s="184" t="s">
+        <v>247</v>
+      </c>
+      <c r="O1" s="185" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B4" s="173" t="s">
-        <v>295</v>
-      </c>
-      <c r="C4" s="173" t="s">
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="172">
+        <v>1</v>
+      </c>
+      <c r="D2" s="174">
+        <v>30</v>
+      </c>
+      <c r="E2" s="172">
+        <f>365*D2/C2</f>
+        <v>10950</v>
+      </c>
+      <c r="F2" s="173">
+        <v>37</v>
+      </c>
+      <c r="G2" s="173">
+        <v>344</v>
+      </c>
+      <c r="H2" s="173">
+        <v>480</v>
+      </c>
+      <c r="I2" s="173">
+        <v>4</v>
+      </c>
+      <c r="J2" s="186">
+        <f>ROUND(I2*H2*G2*F2*E2/1024^3,0)</f>
+        <v>249</v>
+      </c>
+      <c r="K2" s="187">
+        <f>J2*4/1024</f>
+        <v>0.97265625</v>
+      </c>
+      <c r="L2" s="179">
+        <f>365*9/36</f>
+        <v>91.25</v>
+      </c>
+      <c r="M2" s="187">
+        <f>E2/L2</f>
+        <v>120</v>
+      </c>
+      <c r="N2" s="191">
+        <f>M2/24</f>
+        <v>5</v>
+      </c>
+      <c r="O2" s="188">
+        <f>N2/50</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="172">
+        <v>1</v>
+      </c>
+      <c r="D3" s="174">
+        <v>960</v>
+      </c>
+      <c r="E3" s="172">
+        <f>365*D3/C3</f>
+        <v>350400</v>
+      </c>
+      <c r="F3" s="173">
+        <v>37</v>
+      </c>
+      <c r="G3" s="173">
+        <v>344</v>
+      </c>
+      <c r="H3" s="173">
+        <v>480</v>
+      </c>
+      <c r="I3" s="173">
+        <v>4</v>
+      </c>
+      <c r="J3" s="186">
+        <f>ROUND(I3*H3*G3*F3*E3/1024^3,0)</f>
+        <v>7975</v>
+      </c>
+      <c r="K3" s="187">
+        <f>J3*4/1024</f>
+        <v>31.15234375</v>
+      </c>
+      <c r="L3" s="179">
+        <f>L2</f>
+        <v>91.25</v>
+      </c>
+      <c r="M3" s="187">
+        <f>E3/L3</f>
+        <v>3840</v>
+      </c>
+      <c r="N3" s="191">
+        <f t="shared" ref="N3:N5" si="0">M3/24</f>
+        <v>160</v>
+      </c>
+      <c r="O3" s="188">
+        <f>N3/50</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="172">
+        <v>1</v>
+      </c>
+      <c r="D4" s="174">
+        <v>30</v>
+      </c>
+      <c r="E4" s="172">
+        <f>E2</f>
+        <v>10950</v>
+      </c>
+      <c r="F4" s="173">
+        <f t="shared" ref="F4:I5" si="1">F2</f>
+        <v>37</v>
+      </c>
+      <c r="G4" s="173">
+        <v>1126</v>
+      </c>
+      <c r="H4" s="173">
+        <v>1503</v>
+      </c>
+      <c r="I4" s="173">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J4" s="186">
+        <f>ROUND(I4*H4*G4*F4*E4/1024^3,0)</f>
+        <v>2554</v>
+      </c>
+      <c r="K4" s="187">
+        <f>J4*4/1024</f>
+        <v>9.9765625</v>
+      </c>
+      <c r="L4" s="179">
+        <f>L2*G2*H2/G4/H4</f>
+        <v>8.902975576378326</v>
+      </c>
+      <c r="M4" s="187">
+        <f>E4/L4</f>
+        <v>1229.9258720930234</v>
+      </c>
+      <c r="N4" s="191">
+        <f t="shared" si="0"/>
+        <v>51.246911337209305</v>
+      </c>
+      <c r="O4" s="188">
+        <f>N4/50</f>
+        <v>1.024938226744186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="172">
+        <v>1</v>
+      </c>
+      <c r="D5" s="174">
+        <v>960</v>
+      </c>
+      <c r="E5" s="172">
+        <f>E3</f>
+        <v>350400</v>
+      </c>
+      <c r="F5" s="173">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="G5" s="173">
+        <v>1126</v>
+      </c>
+      <c r="H5" s="173">
+        <v>1503</v>
+      </c>
+      <c r="I5" s="173">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="186">
+        <f>ROUND(I5*H5*G5*F5*E5/1024^3,0)</f>
+        <v>81738</v>
+      </c>
+      <c r="K5" s="187">
+        <f>J5*4/1024</f>
+        <v>319.2890625</v>
+      </c>
+      <c r="L5" s="179">
+        <f>L3*G3*H3/G5/H5</f>
+        <v>8.902975576378326</v>
+      </c>
+      <c r="M5" s="187">
+        <f>E5/L5</f>
+        <v>39357.627906976748</v>
+      </c>
+      <c r="N5" s="191">
+        <f t="shared" si="0"/>
+        <v>1639.9011627906978</v>
+      </c>
+      <c r="O5" s="188">
+        <f>N5/50</f>
+        <v>32.798023255813952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="172">
+        <v>1</v>
+      </c>
+      <c r="D6" s="174">
+        <v>8</v>
+      </c>
+      <c r="E6" s="172">
+        <f>365*D6/C6</f>
+        <v>2920</v>
+      </c>
+      <c r="F6" s="173">
+        <v>37</v>
+      </c>
+      <c r="G6" s="173">
+        <v>344</v>
+      </c>
+      <c r="H6" s="173">
+        <v>480</v>
+      </c>
+      <c r="I6" s="173">
+        <v>4</v>
+      </c>
+      <c r="J6" s="186">
+        <f>ROUND(I6*H6*G6*F6*E6/1024^3,0)</f>
+        <v>66</v>
+      </c>
+      <c r="K6" s="187">
+        <f>J6*4/1024</f>
+        <v>0.2578125</v>
+      </c>
+      <c r="L6" s="179">
+        <f>365*9/36</f>
+        <v>91.25</v>
+      </c>
+      <c r="M6" s="187">
+        <f>E6/L6</f>
+        <v>32</v>
+      </c>
+      <c r="N6" s="191">
+        <f>M6/24</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O6" s="188">
+        <f>N6/50</f>
+        <v>2.6666666666666665E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="172"/>
+      <c r="D7" s="174"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="173"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="173"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="182"/>
+      <c r="N7" s="192"/>
+      <c r="O7" s="181"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="172"/>
+      <c r="D8" s="174"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="182"/>
+      <c r="L8" s="179"/>
+      <c r="M8" s="182"/>
+      <c r="N8" s="192"/>
+      <c r="O8" s="181"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="172"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="173"/>
+      <c r="H9" s="173"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="182"/>
+      <c r="L9" s="179"/>
+      <c r="M9" s="182"/>
+      <c r="N9" s="192"/>
+      <c r="O9" s="181"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="172"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="179"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="192"/>
+      <c r="O10" s="181"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="172"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="182"/>
+      <c r="L11" s="179"/>
+      <c r="M11" s="182"/>
+      <c r="N11" s="192"/>
+      <c r="O11" s="181"/>
+    </row>
+    <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="250" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="250"/>
+      <c r="G13" s="250"/>
+      <c r="H13" s="250"/>
+      <c r="I13" s="250"/>
+      <c r="J13" s="250"/>
+      <c r="K13" s="194"/>
+      <c r="L13" s="249" t="s">
+        <v>258</v>
+      </c>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+    </row>
+    <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="175" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="H14" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="I14" s="73" t="s">
+        <v>245</v>
+      </c>
+      <c r="J14" s="189" t="s">
+        <v>249</v>
+      </c>
+      <c r="K14" s="195"/>
+      <c r="L14" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="M14" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="O14" s="73" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>9*365</f>
+        <v>3285</v>
+      </c>
+      <c r="F15">
+        <f>F2</f>
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <f>G2</f>
+        <v>344</v>
+      </c>
+      <c r="H15">
+        <f>H2</f>
+        <v>480</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15" s="186">
+        <f>ROUND(I15*H15*G15*F15*E15/1024^3,1)</f>
+        <v>149.5</v>
+      </c>
+      <c r="L15" s="196">
+        <v>0.99609375</v>
+      </c>
+      <c r="M15" s="180">
+        <v>150</v>
+      </c>
+      <c r="N15" s="180">
+        <v>3473.1</v>
+      </c>
+      <c r="O15" s="178">
+        <f>N15/M15/L15</f>
+        <v>23.244800000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L16" s="196">
+        <v>0.4931640625</v>
+      </c>
+      <c r="M16" s="180">
+        <v>150</v>
+      </c>
+      <c r="N16" s="180">
+        <v>1719.5</v>
+      </c>
+      <c r="O16" s="178">
+        <f t="shared" ref="O16:O17" si="2">N16/M16/L16</f>
+        <v>23.244462046204621</v>
+      </c>
+    </row>
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L17" s="196">
+        <v>0.4931640625</v>
+      </c>
+      <c r="M17" s="180">
         <v>300</v>
       </c>
-      <c r="D4" s="240"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="239">
-        <v>2</v>
-      </c>
-      <c r="B5" s="173" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" s="173" t="s">
-        <v>300</v>
-      </c>
-      <c r="D5" s="240"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="239">
-        <v>3</v>
-      </c>
-      <c r="B6" s="173" t="s">
-        <v>297</v>
-      </c>
-      <c r="C6" s="173" t="s">
-        <v>300</v>
-      </c>
-      <c r="D6" s="240"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="239">
-        <v>4</v>
-      </c>
-      <c r="B7" s="173" t="s">
-        <v>298</v>
-      </c>
-      <c r="C7" s="173" t="s">
-        <v>300</v>
-      </c>
-      <c r="D7" s="240"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="239">
-        <v>5</v>
-      </c>
-      <c r="B8" s="173" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="173" t="s">
-        <v>301</v>
-      </c>
-      <c r="D8" s="240" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="239">
-        <v>6</v>
-      </c>
-      <c r="B9" s="173" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="247" t="s">
-        <v>301</v>
-      </c>
-      <c r="D9" s="240" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="239">
-        <v>7</v>
-      </c>
-      <c r="B10" s="173" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="247" t="s">
-        <v>301</v>
-      </c>
-      <c r="D10" s="240" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="239">
-        <v>8</v>
-      </c>
-      <c r="B11" s="173" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="247" t="s">
-        <v>301</v>
-      </c>
-      <c r="D11" s="240" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="239">
-        <v>9</v>
-      </c>
-      <c r="B12" s="173" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="247" t="s">
-        <v>306</v>
-      </c>
-      <c r="D12" s="240" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="239">
-        <v>10</v>
-      </c>
-      <c r="B13" s="173" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" s="247" t="s">
-        <v>306</v>
-      </c>
-      <c r="D13" s="240" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="239">
-        <v>11</v>
-      </c>
-      <c r="B14" s="173" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="247" t="s">
-        <v>306</v>
-      </c>
-      <c r="D14" s="240" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="239">
-        <v>12</v>
-      </c>
-      <c r="B15" s="173" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" s="247" t="s">
-        <v>300</v>
-      </c>
-      <c r="D15" s="240"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="239">
-        <v>13</v>
-      </c>
-      <c r="B16" s="173" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="247" t="s">
-        <v>300</v>
-      </c>
-      <c r="D16" s="240"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="241">
-        <v>14</v>
-      </c>
-      <c r="B17" s="242" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" s="248" t="s">
-        <v>300</v>
-      </c>
-      <c r="D17" s="243"/>
+      <c r="N17" s="180">
+        <v>3439.1</v>
+      </c>
+      <c r="O17" s="178">
+        <f t="shared" si="2"/>
+        <v>23.245137953795378</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="E13:J13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8123,15 +8462,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E6" sqref="E6"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -9108,14 +9447,14 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6384E697-14DA-42AB-805D-AE9B5B8C5A45}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="E6" sqref="E6"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <selection activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9371,16 +9710,16 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40D0E78-71CC-4A4D-A65A-3E7CBAE30F9C}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E6" sqref="E6"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9593,124 +9932,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F6EE78-61FD-42AC-A045-4FE7AB0E5850}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" style="154" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="152" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" style="152" customWidth="1"/>
-    <col min="4" max="4" width="120.7109375" style="152" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="153"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="151" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="150" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="150" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="150" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="154">
-        <v>1</v>
-      </c>
-      <c r="B2" s="152" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="152" t="s">
-        <v>236</v>
-      </c>
-      <c r="D2" s="152" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="154">
-        <v>2</v>
-      </c>
-      <c r="B3" s="152" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="152" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" s="152" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="154">
-        <v>3</v>
-      </c>
-      <c r="B4" s="152" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="152" t="s">
-        <v>227</v>
-      </c>
-      <c r="D4" s="152" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="154">
-        <v>4</v>
-      </c>
-      <c r="B5" s="152" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" s="152" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="152" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="154">
-        <v>5</v>
-      </c>
-      <c r="B6" s="152" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" s="152" t="s">
-        <v>223</v>
-      </c>
-      <c r="D6" s="152" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="154">
-        <v>6</v>
-      </c>
-      <c r="B7" s="152" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F1DAF-5F35-4965-9F1F-1895AEDF9C0E}">
   <dimension ref="A1:J21"/>
   <sheetViews>
@@ -9859,10 +10080,354 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F6EE78-61FD-42AC-A045-4FE7AB0E5850}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="154" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="152" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" style="152" customWidth="1"/>
+    <col min="4" max="4" width="120.7109375" style="152" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="153"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="151" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="150" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="150" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="150" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="154">
+        <v>1</v>
+      </c>
+      <c r="B2" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="152" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="152" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="154">
+        <v>2</v>
+      </c>
+      <c r="B3" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="152" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="152" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="154">
+        <v>3</v>
+      </c>
+      <c r="B4" s="152" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="152" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="152" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="154">
+        <v>4</v>
+      </c>
+      <c r="B5" s="152" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="152" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="152" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="154">
+        <v>5</v>
+      </c>
+      <c r="B6" s="152" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="152" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="152" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="154">
+        <v>6</v>
+      </c>
+      <c r="B7" s="152" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9E9723-48CB-44D6-9690-AF1878CFBFAF}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="159.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="244" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="245" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="245" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="246" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="239">
+        <v>1</v>
+      </c>
+      <c r="B4" s="173" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="173" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="240"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="239">
+        <v>2</v>
+      </c>
+      <c r="B5" s="173" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" s="173" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="240"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="239">
+        <v>3</v>
+      </c>
+      <c r="B6" s="173" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="173" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="240"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="239">
+        <v>4</v>
+      </c>
+      <c r="B7" s="173" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="173" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="240"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="239">
+        <v>5</v>
+      </c>
+      <c r="B8" s="173" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="173" t="s">
+        <v>301</v>
+      </c>
+      <c r="D8" s="240" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="239">
+        <v>6</v>
+      </c>
+      <c r="B9" s="173" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="247" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" s="240" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="239">
+        <v>7</v>
+      </c>
+      <c r="B10" s="173" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="247" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10" s="240" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="239">
+        <v>8</v>
+      </c>
+      <c r="B11" s="173" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="247" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="240" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="239">
+        <v>9</v>
+      </c>
+      <c r="B12" s="173" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="247" t="s">
+        <v>306</v>
+      </c>
+      <c r="D12" s="240" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="239">
+        <v>10</v>
+      </c>
+      <c r="B13" s="173" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="247" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" s="240" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="239">
+        <v>11</v>
+      </c>
+      <c r="B14" s="173" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="247" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="240" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="239">
+        <v>12</v>
+      </c>
+      <c r="B15" s="173" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="247" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="240"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="239">
+        <v>13</v>
+      </c>
+      <c r="B16" s="173" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="247" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="240"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="241">
+        <v>14</v>
+      </c>
+      <c r="B17" s="242" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="248" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="243"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87BC478-B255-4AE7-8F80-4F329E7A5E8D}">
   <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
+    <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -9897,566 +10462,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873E6B2-35C4-4A79-9D06-5BB2CD1E5FA3}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:O17"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="180"/>
-    <col min="12" max="12" width="9.28515625" style="180" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="180"/>
-    <col min="15" max="15" width="9.140625" style="178"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="177" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="175" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="176" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1" s="175" t="s">
-        <v>242</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="J1" s="189" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="190" t="s">
-        <v>250</v>
-      </c>
-      <c r="L1" s="183" t="s">
-        <v>248</v>
-      </c>
-      <c r="M1" s="184" t="s">
-        <v>246</v>
-      </c>
-      <c r="N1" s="184" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="185" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="172">
-        <v>1</v>
-      </c>
-      <c r="D2" s="174">
-        <v>30</v>
-      </c>
-      <c r="E2" s="172">
-        <f>365*D2/C2</f>
-        <v>10950</v>
-      </c>
-      <c r="F2" s="173">
-        <v>37</v>
-      </c>
-      <c r="G2" s="173">
-        <v>344</v>
-      </c>
-      <c r="H2" s="173">
-        <v>480</v>
-      </c>
-      <c r="I2" s="173">
-        <v>4</v>
-      </c>
-      <c r="J2" s="186">
-        <f>ROUND(I2*H2*G2*F2*E2/1024^3,0)</f>
-        <v>249</v>
-      </c>
-      <c r="K2" s="187">
-        <f>J2*4/1024</f>
-        <v>0.97265625</v>
-      </c>
-      <c r="L2" s="179">
-        <f>365*9/36</f>
-        <v>91.25</v>
-      </c>
-      <c r="M2" s="187">
-        <f>E2/L2</f>
-        <v>120</v>
-      </c>
-      <c r="N2" s="191">
-        <f>M2/24</f>
-        <v>5</v>
-      </c>
-      <c r="O2" s="188">
-        <f>N2/50</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="172">
-        <v>1</v>
-      </c>
-      <c r="D3" s="174">
-        <v>960</v>
-      </c>
-      <c r="E3" s="172">
-        <f>365*D3/C3</f>
-        <v>350400</v>
-      </c>
-      <c r="F3" s="173">
-        <v>37</v>
-      </c>
-      <c r="G3" s="173">
-        <v>344</v>
-      </c>
-      <c r="H3" s="173">
-        <v>480</v>
-      </c>
-      <c r="I3" s="173">
-        <v>4</v>
-      </c>
-      <c r="J3" s="186">
-        <f>ROUND(I3*H3*G3*F3*E3/1024^3,0)</f>
-        <v>7975</v>
-      </c>
-      <c r="K3" s="187">
-        <f>J3*4/1024</f>
-        <v>31.15234375</v>
-      </c>
-      <c r="L3" s="179">
-        <f>L2</f>
-        <v>91.25</v>
-      </c>
-      <c r="M3" s="187">
-        <f>E3/L3</f>
-        <v>3840</v>
-      </c>
-      <c r="N3" s="191">
-        <f t="shared" ref="N3:N5" si="0">M3/24</f>
-        <v>160</v>
-      </c>
-      <c r="O3" s="188">
-        <f>N3/50</f>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" s="172">
-        <v>1</v>
-      </c>
-      <c r="D4" s="174">
-        <v>30</v>
-      </c>
-      <c r="E4" s="172">
-        <f>E2</f>
-        <v>10950</v>
-      </c>
-      <c r="F4" s="173">
-        <f t="shared" ref="F4:I5" si="1">F2</f>
-        <v>37</v>
-      </c>
-      <c r="G4" s="173">
-        <v>1126</v>
-      </c>
-      <c r="H4" s="173">
-        <v>1503</v>
-      </c>
-      <c r="I4" s="173">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J4" s="186">
-        <f>ROUND(I4*H4*G4*F4*E4/1024^3,0)</f>
-        <v>2554</v>
-      </c>
-      <c r="K4" s="187">
-        <f>J4*4/1024</f>
-        <v>9.9765625</v>
-      </c>
-      <c r="L4" s="179">
-        <f>L2*G2*H2/G4/H4</f>
-        <v>8.902975576378326</v>
-      </c>
-      <c r="M4" s="187">
-        <f>E4/L4</f>
-        <v>1229.9258720930234</v>
-      </c>
-      <c r="N4" s="191">
-        <f t="shared" si="0"/>
-        <v>51.246911337209305</v>
-      </c>
-      <c r="O4" s="188">
-        <f>N4/50</f>
-        <v>1.024938226744186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" s="172">
-        <v>1</v>
-      </c>
-      <c r="D5" s="174">
-        <v>960</v>
-      </c>
-      <c r="E5" s="172">
-        <f>E3</f>
-        <v>350400</v>
-      </c>
-      <c r="F5" s="173">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="G5" s="173">
-        <v>1126</v>
-      </c>
-      <c r="H5" s="173">
-        <v>1503</v>
-      </c>
-      <c r="I5" s="173">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J5" s="186">
-        <f>ROUND(I5*H5*G5*F5*E5/1024^3,0)</f>
-        <v>81738</v>
-      </c>
-      <c r="K5" s="187">
-        <f>J5*4/1024</f>
-        <v>319.2890625</v>
-      </c>
-      <c r="L5" s="179">
-        <f>L3*G3*H3/G5/H5</f>
-        <v>8.902975576378326</v>
-      </c>
-      <c r="M5" s="187">
-        <f>E5/L5</f>
-        <v>39357.627906976748</v>
-      </c>
-      <c r="N5" s="191">
-        <f t="shared" si="0"/>
-        <v>1639.9011627906978</v>
-      </c>
-      <c r="O5" s="188">
-        <f>N5/50</f>
-        <v>32.798023255813952</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C6" s="172">
-        <v>1</v>
-      </c>
-      <c r="D6" s="174">
-        <v>8</v>
-      </c>
-      <c r="E6" s="172">
-        <f>365*D6/C6</f>
-        <v>2920</v>
-      </c>
-      <c r="F6" s="173">
-        <v>37</v>
-      </c>
-      <c r="G6" s="173">
-        <v>344</v>
-      </c>
-      <c r="H6" s="173">
-        <v>480</v>
-      </c>
-      <c r="I6" s="173">
-        <v>4</v>
-      </c>
-      <c r="J6" s="186">
-        <f>ROUND(I6*H6*G6*F6*E6/1024^3,0)</f>
-        <v>66</v>
-      </c>
-      <c r="K6" s="187">
-        <f>J6*4/1024</f>
-        <v>0.2578125</v>
-      </c>
-      <c r="L6" s="179">
-        <f>365*9/36</f>
-        <v>91.25</v>
-      </c>
-      <c r="M6" s="187">
-        <f>E6/L6</f>
-        <v>32</v>
-      </c>
-      <c r="N6" s="191">
-        <f>M6/24</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="O6" s="188">
-        <f>N6/50</f>
-        <v>2.6666666666666665E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="174"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="173"/>
-      <c r="H7" s="173"/>
-      <c r="I7" s="173"/>
-      <c r="J7" s="173"/>
-      <c r="K7" s="182"/>
-      <c r="L7" s="179"/>
-      <c r="M7" s="182"/>
-      <c r="N7" s="192"/>
-      <c r="O7" s="181"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="172"/>
-      <c r="D8" s="174"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="173"/>
-      <c r="H8" s="173"/>
-      <c r="I8" s="173"/>
-      <c r="J8" s="173"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="179"/>
-      <c r="M8" s="182"/>
-      <c r="N8" s="192"/>
-      <c r="O8" s="181"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="172"/>
-      <c r="D9" s="174"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="173"/>
-      <c r="H9" s="173"/>
-      <c r="I9" s="173"/>
-      <c r="J9" s="173"/>
-      <c r="K9" s="182"/>
-      <c r="L9" s="179"/>
-      <c r="M9" s="182"/>
-      <c r="N9" s="192"/>
-      <c r="O9" s="181"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="172"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="173"/>
-      <c r="H10" s="173"/>
-      <c r="I10" s="173"/>
-      <c r="J10" s="173"/>
-      <c r="K10" s="182"/>
-      <c r="L10" s="179"/>
-      <c r="M10" s="182"/>
-      <c r="N10" s="192"/>
-      <c r="O10" s="181"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="172"/>
-      <c r="D11" s="174"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="173"/>
-      <c r="H11" s="173"/>
-      <c r="I11" s="173"/>
-      <c r="J11" s="173"/>
-      <c r="K11" s="182"/>
-      <c r="L11" s="179"/>
-      <c r="M11" s="182"/>
-      <c r="N11" s="192"/>
-      <c r="O11" s="181"/>
-    </row>
-    <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="250" t="s">
-        <v>263</v>
-      </c>
-      <c r="F13" s="250"/>
-      <c r="G13" s="250"/>
-      <c r="H13" s="250"/>
-      <c r="I13" s="250"/>
-      <c r="J13" s="250"/>
-      <c r="K13" s="194"/>
-      <c r="L13" s="249" t="s">
-        <v>258</v>
-      </c>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
-    </row>
-    <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="175" t="s">
-        <v>242</v>
-      </c>
-      <c r="F14" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="G14" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="H14" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="I14" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="J14" s="189" t="s">
-        <v>249</v>
-      </c>
-      <c r="K14" s="195"/>
-      <c r="L14" s="73" t="s">
-        <v>262</v>
-      </c>
-      <c r="M14" s="73" t="s">
-        <v>259</v>
-      </c>
-      <c r="N14" s="73" t="s">
-        <v>260</v>
-      </c>
-      <c r="O14" s="73" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <f>9*365</f>
-        <v>3285</v>
-      </c>
-      <c r="F15">
-        <f>F2</f>
-        <v>37</v>
-      </c>
-      <c r="G15">
-        <f>G2</f>
-        <v>344</v>
-      </c>
-      <c r="H15">
-        <f>H2</f>
-        <v>480</v>
-      </c>
-      <c r="I15">
-        <v>8</v>
-      </c>
-      <c r="J15" s="186">
-        <f>ROUND(I15*H15*G15*F15*E15/1024^3,1)</f>
-        <v>149.5</v>
-      </c>
-      <c r="L15" s="196">
-        <v>0.99609375</v>
-      </c>
-      <c r="M15" s="180">
-        <v>150</v>
-      </c>
-      <c r="N15" s="180">
-        <v>3473.1</v>
-      </c>
-      <c r="O15" s="178">
-        <f>N15/M15/L15</f>
-        <v>23.244800000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L16" s="196">
-        <v>0.4931640625</v>
-      </c>
-      <c r="M16" s="180">
-        <v>150</v>
-      </c>
-      <c r="N16" s="180">
-        <v>1719.5</v>
-      </c>
-      <c r="O16" s="178">
-        <f t="shared" ref="O16:O17" si="2">N16/M16/L16</f>
-        <v>23.244462046204621</v>
-      </c>
-    </row>
-    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L17" s="196">
-        <v>0.4931640625</v>
-      </c>
-      <c r="M17" s="180">
-        <v>300</v>
-      </c>
-      <c r="N17" s="180">
-        <v>3439.1</v>
-      </c>
-      <c r="O17" s="178">
-        <f t="shared" si="2"/>
-        <v>23.245137953795378</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="E13:J13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
PRJ -> imod python. 1st attempt.
Haven't succeeded with this yet. Commiting to test some things
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1007" documentId="13_ncr:1_{7A66306F-20CB-4569-A9D0-64235774BF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78ED0F2A-009B-49A0-9711-02D9C8305B74}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8FE4554C-EB24-43D3-9010-76DE7A8D1AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4E6CC52-C0C4-432B-B951-4263F9BCA6A1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -593,6 +593,24 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={E42EC14D-BD5A-400D-A934-346EA61A0CA2}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check source code for more.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={8E0E0613-5620-4CD4-A681-6187F9B32A6D}</author>
     <author>tc={4C755D57-E80D-4678-A151-E00B776F1F03}</author>
     <author>tc={93547DE0-9536-496B-8566-6EFCF9FF2A35}</author>
@@ -646,7 +664,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="316">
   <si>
     <t>#</t>
   </si>
@@ -2325,6 +2343,24 @@
   <si>
     <t>He didn't even mention it in his email.</t>
   </si>
+  <si>
+    <t>imod.formats.prj.open_projectfile_data</t>
+  </si>
+  <si>
+    <t>imod python bugs/potential improvements:</t>
+  </si>
+  <si>
+    <t>loading imod takes an eternity. Modularizing it would fix that.</t>
+  </si>
+  <si>
+    <t>It's modularized, but a lot of modules use import imod instead of importing specific libraries, which makes it much slower.</t>
+  </si>
+  <si>
+    <t>doesn't return dictionary, but tuple. First item is the dict, second item is the period_data dict.</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
 </sst>
 </file>
 
@@ -2333,7 +2369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2470,6 +2506,13 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3096,7 +3139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="262">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3778,6 +3821,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3908,58 +3960,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>255930</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>113833</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B04434-7855-49DD-B4FC-C3BBC62C08ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="657225" y="0"/>
-          <a:ext cx="9961905" cy="3733333"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>494326</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>46718</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3976,7 +3984,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3985,6 +3993,50 @@
         <a:xfrm>
           <a:off x="628650" y="4410075"/>
           <a:ext cx="7790476" cy="7257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2721581</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>46614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1EF6E1-BE1C-F82F-0DFD-FFCA9B35F01F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="8458200"/>
+          <a:ext cx="13732481" cy="7590414"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4547,6 +4599,14 @@
 
 <file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q2" dT="2025-07-15T09:17:30.76" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
+    <text>Check source code for more.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="J1" dT="2025-04-25T10:51:09.87" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{8E0E0613-5620-4CD4-A681-6187F9B32A6D}">
     <text>Just for the .HED file</text>
   </threadedComment>
@@ -5030,21 +5090,21 @@
       <c r="O11" s="181"/>
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="250" t="s">
+      <c r="E13" s="253" t="s">
         <v>263</v>
       </c>
-      <c r="F13" s="250"/>
-      <c r="G13" s="250"/>
-      <c r="H13" s="250"/>
-      <c r="I13" s="250"/>
-      <c r="J13" s="250"/>
+      <c r="F13" s="253"/>
+      <c r="G13" s="253"/>
+      <c r="H13" s="253"/>
+      <c r="I13" s="253"/>
+      <c r="J13" s="253"/>
       <c r="K13" s="194"/>
-      <c r="L13" s="249" t="s">
+      <c r="L13" s="252" t="s">
         <v>258</v>
       </c>
-      <c r="M13" s="249"/>
-      <c r="N13" s="249"/>
-      <c r="O13" s="249"/>
+      <c r="M13" s="252"/>
+      <c r="N13" s="252"/>
+      <c r="O13" s="252"/>
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">
@@ -5224,50 +5284,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="257" t="s">
+      <c r="B6" s="260" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="258"/>
-      <c r="D6" s="258"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="259" t="s">
+      <c r="F6" s="262" t="s">
         <v>287</v>
       </c>
-      <c r="G6" s="259"/>
-      <c r="H6" s="259"/>
-      <c r="I6" s="259"/>
-      <c r="J6" s="259"/>
+      <c r="G6" s="262"/>
+      <c r="H6" s="262"/>
+      <c r="I6" s="262"/>
+      <c r="J6" s="262"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="258" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="256"/>
-      <c r="D7" s="256"/>
+      <c r="C7" s="259"/>
+      <c r="D7" s="259"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="254" t="s">
+      <c r="F7" s="257" t="s">
         <v>274</v>
       </c>
-      <c r="G7" s="254"/>
-      <c r="H7" s="254"/>
-      <c r="I7" s="254"/>
-      <c r="J7" s="254"/>
+      <c r="G7" s="257"/>
+      <c r="H7" s="257"/>
+      <c r="I7" s="257"/>
+      <c r="J7" s="257"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="251" t="s">
+      <c r="B8" s="254" t="s">
         <v>290</v>
       </c>
-      <c r="C8" s="252"/>
+      <c r="C8" s="255"/>
       <c r="D8" s="225" t="s">
         <v>277</v>
       </c>
       <c r="E8" s="210"/>
-      <c r="F8" s="253" t="s">
+      <c r="F8" s="256" t="s">
         <v>290</v>
       </c>
-      <c r="G8" s="253"/>
+      <c r="G8" s="256"/>
       <c r="H8" s="232" t="s">
         <v>277</v>
       </c>
@@ -6582,50 +6642,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="257" t="s">
+      <c r="B6" s="260" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="258"/>
-      <c r="D6" s="258"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="259" t="s">
+      <c r="F6" s="262" t="s">
         <v>287</v>
       </c>
-      <c r="G6" s="259"/>
-      <c r="H6" s="259"/>
-      <c r="I6" s="259"/>
-      <c r="J6" s="259"/>
+      <c r="G6" s="262"/>
+      <c r="H6" s="262"/>
+      <c r="I6" s="262"/>
+      <c r="J6" s="262"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="258" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="256"/>
-      <c r="D7" s="256"/>
+      <c r="C7" s="259"/>
+      <c r="D7" s="259"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="254" t="s">
+      <c r="F7" s="257" t="s">
         <v>274</v>
       </c>
-      <c r="G7" s="254"/>
-      <c r="H7" s="254"/>
-      <c r="I7" s="254"/>
-      <c r="J7" s="254"/>
+      <c r="G7" s="257"/>
+      <c r="H7" s="257"/>
+      <c r="I7" s="257"/>
+      <c r="J7" s="257"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="260" t="s">
+      <c r="B8" s="263" t="s">
         <v>290</v>
       </c>
-      <c r="C8" s="261"/>
+      <c r="C8" s="264"/>
       <c r="D8" s="236" t="s">
         <v>277</v>
       </c>
       <c r="E8" s="209"/>
-      <c r="F8" s="253" t="s">
+      <c r="F8" s="256" t="s">
         <v>290</v>
       </c>
-      <c r="G8" s="253"/>
+      <c r="G8" s="256"/>
       <c r="H8" s="232" t="s">
         <v>277</v>
       </c>
@@ -10205,7 +10265,7 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -10425,41 +10485,72 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87BC478-B255-4AE7-8F80-4F329E7A5E8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87BC478-B255-4AE7-8F80-4F329E7A5E8D}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="15" width="9.140625" style="249"/>
+    <col min="16" max="16" width="37.140625" style="249" customWidth="1"/>
+    <col min="17" max="17" width="76.5703125" style="144" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="249"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="249">
+        <v>2</v>
+      </c>
+      <c r="B1" s="249" t="s">
+        <v>237</v>
+      </c>
+      <c r="O1" s="250" t="s">
+        <v>311</v>
+      </c>
+      <c r="P1" s="250" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q1" s="251" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="O2" s="250">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="P2" s="250" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q2" s="251" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="249">
+        <v>3</v>
+      </c>
+      <c r="B3" s="249" t="s">
+        <v>238</v>
+      </c>
+      <c r="O3" s="250">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>238</v>
+      <c r="P3" s="250" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q3" s="251" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Routine: pre imod_python_init_NBr31.ipynb changes.
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB2663B3-CF85-4E29-B74B-672DB375EEE7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,7 +596,7 @@
     <author>tc={E42EC14D-BD5A-400D-A934-346EA61A0CA2}</author>
   </authors>
   <commentList>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -664,7 +664,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="321">
   <si>
     <t>#</t>
   </si>
@@ -2088,12 +2088,6 @@
     </r>
   </si>
   <si>
-    <t>Can't read OBS file (I had to make a my modified function to read a PRJ file with OBS)</t>
-  </si>
-  <si>
-    <t>SHD array cannot have nan values, even when the layer thickness is 0 (so those cells become innactive) for some reason.</t>
-  </si>
-  <si>
     <t>Layers</t>
   </si>
   <si>
@@ -2367,6 +2361,21 @@
   <si>
     <t>I think time should be discarted in this case.</t>
   </si>
+  <si>
+    <t>Screenshots related to bugs</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Image #</t>
+  </si>
+  <si>
+    <t>Sentence of coupler documentation doesn't make sense.</t>
+  </si>
+  <si>
+    <t>Chech screenshot</t>
+  </si>
 </sst>
 </file>
 
@@ -2375,7 +2384,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2517,6 +2526,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -3145,7 +3162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3874,6 +3891,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3965,23 +3997,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>494326</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>46718</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>254606</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>179964</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2516E69E-445A-43A3-E91B-36F40D5EAD3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1EF6E1-BE1C-F82F-0DFD-FFCA9B35F01F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3997,8 +4029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="4410075"/>
-          <a:ext cx="7790476" cy="7257143"/>
+          <a:off x="9753600" y="5753100"/>
+          <a:ext cx="13732481" cy="7590414"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4009,23 +4041,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7895</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>2721581</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>46614</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>45314</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>151528</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1EF6E1-BE1C-F82F-0DFD-FFCA9B35F01F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE91B021-F66D-96E3-DA22-19808AEEA1AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4041,52 +4073,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="8458200"/>
-          <a:ext cx="13732481" cy="7590414"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>531090</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>113428</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE91B021-F66D-96E3-DA22-19808AEEA1AA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9144000" y="1143000"/>
-          <a:ext cx="18476190" cy="6971428"/>
+          <a:off x="9744075" y="588920"/>
+          <a:ext cx="13532714" cy="5106158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4649,7 +4637,7 @@
 
 <file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="Q2" dT="2025-07-15T09:17:30.76" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
+  <threadedComment ref="D3" dT="2025-07-15T09:17:30.76" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
     <text>Check source code for more.</text>
   </threadedComment>
 </ThreadedComments>
@@ -4733,46 +4721,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="175" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="176" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" s="175" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="73" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="J1" s="189" t="s">
+        <v>247</v>
+      </c>
+      <c r="K1" s="190" t="s">
+        <v>248</v>
+      </c>
+      <c r="L1" s="183" t="s">
+        <v>246</v>
+      </c>
+      <c r="M1" s="184" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="176" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1" s="175" t="s">
-        <v>242</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" s="73" t="s">
+      <c r="N1" s="184" t="s">
         <v>245</v>
       </c>
-      <c r="J1" s="189" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="190" t="s">
+      <c r="O1" s="185" t="s">
         <v>250</v>
-      </c>
-      <c r="L1" s="183" t="s">
-        <v>248</v>
-      </c>
-      <c r="M1" s="184" t="s">
-        <v>246</v>
-      </c>
-      <c r="N1" s="184" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="185" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4780,7 +4768,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C2" s="172">
         <v>1</v>
@@ -4834,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C3" s="172">
         <v>1</v>
@@ -4888,7 +4876,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C4" s="172">
         <v>1</v>
@@ -4944,7 +4932,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" s="172">
         <v>1</v>
@@ -5000,7 +4988,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C6" s="172">
         <v>1</v>
@@ -5141,7 +5129,7 @@
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E13" s="253" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F13" s="253"/>
       <c r="G13" s="253"/>
@@ -5150,7 +5138,7 @@
       <c r="J13" s="253"/>
       <c r="K13" s="194"/>
       <c r="L13" s="252" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M13" s="252"/>
       <c r="N13" s="252"/>
@@ -5158,35 +5146,35 @@
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F14" s="73" t="s">
+        <v>237</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" s="73" t="s">
         <v>239</v>
       </c>
-      <c r="G14" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="H14" s="73" t="s">
-        <v>241</v>
-      </c>
       <c r="I14" s="73" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="73" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M14" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="O14" s="73" t="s">
         <v>259</v>
-      </c>
-      <c r="N14" s="73" t="s">
-        <v>260</v>
-      </c>
-      <c r="O14" s="73" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5297,7 +5285,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="198" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D1" s="223"/>
       <c r="F1" s="212"/>
@@ -5308,7 +5296,7 @@
     </row>
     <row r="2" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="198" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D2" s="223"/>
       <c r="F2" s="212"/>
@@ -5319,7 +5307,7 @@
     </row>
     <row r="4" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="198" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D4" s="223"/>
       <c r="F4" s="212"/>
@@ -5330,18 +5318,18 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="198" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="260" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C6" s="261"/>
       <c r="D6" s="261"/>
       <c r="E6" s="211"/>
       <c r="F6" s="262" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G6" s="262"/>
       <c r="H6" s="262"/>
@@ -5351,13 +5339,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="258" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" s="259"/>
       <c r="D7" s="259"/>
       <c r="E7" s="209"/>
       <c r="F7" s="257" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="257"/>
       <c r="H7" s="257"/>
@@ -5367,41 +5355,41 @@
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="254" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C8" s="255"/>
       <c r="D8" s="225" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E8" s="210"/>
       <c r="F8" s="256" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G8" s="256"/>
       <c r="H8" s="232" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I8" s="232" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J8" s="218" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K8" s="237"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="199" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C9" s="200"/>
       <c r="D9" s="226"/>
       <c r="E9" s="201" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F9" s="214"/>
       <c r="G9" s="214"/>
       <c r="H9" s="233" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I9" s="233"/>
       <c r="J9" s="219"/>
@@ -5409,17 +5397,17 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="199" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="200"/>
       <c r="D10" s="226"/>
       <c r="E10" s="201" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F10" s="214"/>
       <c r="G10" s="214"/>
       <c r="H10" s="233" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I10" s="233"/>
       <c r="J10" s="219"/>
@@ -5427,20 +5415,20 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="199" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C11" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D11" s="226">
         <v>85372.449299999993</v>
       </c>
       <c r="E11" s="201"/>
       <c r="F11" s="214" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G11" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H11" s="233">
         <v>85372.449299999993</v>
@@ -5457,20 +5445,20 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C12" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D12" s="226">
         <v>0</v>
       </c>
       <c r="E12" s="201"/>
       <c r="F12" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G12" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H12" s="233">
         <v>0</v>
@@ -5487,20 +5475,20 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C13" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D13" s="226">
         <v>0</v>
       </c>
       <c r="E13" s="201"/>
       <c r="F13" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G13" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H13" s="233">
         <v>0</v>
@@ -5517,20 +5505,20 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C14" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D14" s="226">
         <v>0</v>
       </c>
       <c r="E14" s="201"/>
       <c r="F14" s="214" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G14" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H14" s="233">
         <v>0</v>
@@ -5547,20 +5535,20 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C15" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D15" s="226">
         <v>1.1268</v>
       </c>
       <c r="E15" s="201"/>
       <c r="F15" s="214" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G15" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H15" s="233">
         <v>1.1268</v>
@@ -5577,20 +5565,20 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="199" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C16" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D16" s="226">
         <v>730030.94590000005</v>
       </c>
       <c r="E16" s="201"/>
       <c r="F16" s="214" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G16" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H16" s="233">
         <v>730030.94590000005</v>
@@ -5610,7 +5598,7 @@
         <v>214</v>
       </c>
       <c r="C17" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D17" s="226">
         <v>49526.385000000002</v>
@@ -5620,7 +5608,7 @@
         <v>214</v>
       </c>
       <c r="G17" s="213" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H17" s="233">
         <v>49526.385000000002</v>
@@ -5641,10 +5629,10 @@
       <c r="D18" s="226"/>
       <c r="E18" s="201"/>
       <c r="F18" s="214" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G18" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H18" s="233">
         <v>0</v>
@@ -5667,20 +5655,20 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="205" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C20" s="206" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D20" s="228">
         <v>864930.90700000001</v>
       </c>
       <c r="E20" s="207"/>
       <c r="F20" s="221" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G20" s="221" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H20" s="234">
         <v>864930.90700000001</v>
@@ -5697,18 +5685,18 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="199" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C21" s="200" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D21" s="226"/>
       <c r="E21" s="201"/>
       <c r="F21" s="214" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G21" s="214" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H21" s="233"/>
       <c r="I21" s="233"/>
@@ -5717,18 +5705,18 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="199" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C22" s="200" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D22" s="226"/>
       <c r="E22" s="201"/>
       <c r="F22" s="214" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G22" s="214" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H22" s="233"/>
       <c r="I22" s="233"/>
@@ -5737,20 +5725,20 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="199" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C23" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D23" s="226">
         <v>628508.89240000001</v>
       </c>
       <c r="E23" s="201"/>
       <c r="F23" s="214" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G23" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H23" s="233">
         <v>628508.89240000001</v>
@@ -5767,20 +5755,20 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C24" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D24" s="226">
         <v>30344.652300000002</v>
       </c>
       <c r="E24" s="201"/>
       <c r="F24" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G24" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H24" s="233">
         <v>30344.652300000002</v>
@@ -5797,20 +5785,20 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C25" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D25" s="226">
         <v>3355.8359</v>
       </c>
       <c r="E25" s="201"/>
       <c r="F25" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G25" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H25" s="233">
         <v>3355.8359</v>
@@ -5827,20 +5815,20 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C26" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D26" s="226">
         <v>26518.071100000001</v>
       </c>
       <c r="E26" s="201"/>
       <c r="F26" s="214" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G26" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H26" s="233">
         <v>26518.071100000001</v>
@@ -5857,20 +5845,20 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C27" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D27" s="226">
         <v>31860.243399999999</v>
       </c>
       <c r="E27" s="201"/>
       <c r="F27" s="214" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G27" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H27" s="233">
         <v>31860.243399999999</v>
@@ -5887,20 +5875,20 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="199" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C28" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D28" s="226">
         <v>75077.154500000004</v>
       </c>
       <c r="E28" s="201"/>
       <c r="F28" s="214" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G28" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H28" s="233">
         <v>75077.154500000004</v>
@@ -5920,7 +5908,7 @@
         <v>214</v>
       </c>
       <c r="C29" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D29" s="226">
         <v>69409.986699999994</v>
@@ -5930,7 +5918,7 @@
         <v>214</v>
       </c>
       <c r="G29" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H29" s="233">
         <v>69409.986699999994</v>
@@ -5945,10 +5933,10 @@
       <c r="D30" s="226"/>
       <c r="E30" s="201"/>
       <c r="F30" s="214" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G30" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H30" s="233">
         <v>0</v>
@@ -5971,20 +5959,20 @@
     </row>
     <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="202" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C32" s="203" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D32" s="229">
         <v>865074.83640000003</v>
       </c>
       <c r="E32" s="204"/>
       <c r="F32" s="215" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G32" s="215" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H32" s="235">
         <v>865074.83640000003</v>
@@ -6023,7 +6011,7 @@
     </row>
     <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="238" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B35" s="200"/>
       <c r="C35" s="200"/>
@@ -6655,7 +6643,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="198" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D1" s="223"/>
       <c r="F1" s="212"/>
@@ -6666,7 +6654,7 @@
     </row>
     <row r="2" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="198" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D2" s="223"/>
       <c r="F2" s="212"/>
@@ -6677,7 +6665,7 @@
     </row>
     <row r="4" spans="1:11" s="198" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="198" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D4" s="223"/>
       <c r="F4" s="212"/>
@@ -6688,18 +6676,18 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="198" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="260" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C6" s="261"/>
       <c r="D6" s="261"/>
       <c r="E6" s="211"/>
       <c r="F6" s="262" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G6" s="262"/>
       <c r="H6" s="262"/>
@@ -6709,13 +6697,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="258" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" s="259"/>
       <c r="D7" s="259"/>
       <c r="E7" s="209"/>
       <c r="F7" s="257" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="257"/>
       <c r="H7" s="257"/>
@@ -6725,41 +6713,41 @@
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="263" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C8" s="264"/>
       <c r="D8" s="236" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E8" s="209"/>
       <c r="F8" s="256" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G8" s="256"/>
       <c r="H8" s="232" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I8" s="232" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J8" s="218" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K8" s="237"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="199" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C9" s="200"/>
       <c r="D9" s="226"/>
       <c r="E9" s="201" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F9" s="214"/>
       <c r="G9" s="214"/>
       <c r="H9" s="233" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I9" s="233"/>
       <c r="J9" s="219"/>
@@ -6767,17 +6755,17 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="199" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="200"/>
       <c r="D10" s="226"/>
       <c r="E10" s="201" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F10" s="214"/>
       <c r="G10" s="214"/>
       <c r="H10" s="233" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I10" s="233"/>
       <c r="J10" s="219"/>
@@ -6785,20 +6773,20 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="199" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C11" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D11" s="226">
         <v>85372.449299999993</v>
       </c>
       <c r="E11" s="201"/>
       <c r="F11" s="214" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G11" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H11" s="233">
         <v>82156.388500000001</v>
@@ -6815,20 +6803,20 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C12" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D12" s="226">
         <v>0</v>
       </c>
       <c r="E12" s="201"/>
       <c r="F12" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G12" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H12" s="233">
         <v>0</v>
@@ -6839,20 +6827,20 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C13" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D13" s="226">
         <v>0</v>
       </c>
       <c r="E13" s="201"/>
       <c r="F13" s="214" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G13" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H13" s="233">
         <v>0</v>
@@ -6863,20 +6851,20 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C14" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D14" s="226">
         <v>0</v>
       </c>
       <c r="E14" s="201"/>
       <c r="F14" s="214" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G14" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H14" s="233">
         <v>1.1268</v>
@@ -6893,20 +6881,20 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C15" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D15" s="226">
         <v>0</v>
       </c>
       <c r="E15" s="201"/>
       <c r="F15" s="214" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G15" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H15" s="233">
         <v>730016.60699999996</v>
@@ -6923,10 +6911,10 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C16" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D16" s="226">
         <v>0</v>
@@ -6936,7 +6924,7 @@
         <v>214</v>
       </c>
       <c r="G16" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H16" s="233">
         <v>47252.058599999997</v>
@@ -6953,20 +6941,20 @@
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C17" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D17" s="226">
         <v>0</v>
       </c>
       <c r="E17" s="201"/>
       <c r="F17" s="214" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G17" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H17" s="233">
         <v>0</v>
@@ -6977,10 +6965,10 @@
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C18" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D18" s="226">
         <v>0</v>
@@ -6995,20 +6983,20 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C19" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D19" s="226">
         <v>0</v>
       </c>
       <c r="E19" s="201"/>
       <c r="F19" s="214" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G19" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H19" s="233">
         <v>859426.18099999998</v>
@@ -7025,10 +7013,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C20" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D20" s="226">
         <v>0</v>
@@ -7043,10 +7031,10 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C21" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D21" s="226">
         <v>0</v>
@@ -7061,10 +7049,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C22" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D22" s="226">
         <v>0</v>
@@ -7079,10 +7067,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C23" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D23" s="226">
         <v>1.1268</v>
@@ -7097,10 +7085,10 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="199" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C24" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D24" s="226">
         <v>730030.94590000005</v>
@@ -7118,7 +7106,7 @@
         <v>214</v>
       </c>
       <c r="C25" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D25" s="226">
         <v>530.32600000000002</v>
@@ -7136,7 +7124,7 @@
         <v>214</v>
       </c>
       <c r="C26" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D26" s="226">
         <v>3913.6963000000001</v>
@@ -7154,7 +7142,7 @@
         <v>214</v>
       </c>
       <c r="C27" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D27" s="226">
         <v>2842.8613</v>
@@ -7172,7 +7160,7 @@
         <v>214</v>
       </c>
       <c r="C28" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D28" s="226">
         <v>1014.8166</v>
@@ -7190,7 +7178,7 @@
         <v>214</v>
       </c>
       <c r="C29" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D29" s="226">
         <v>778.73800000000006</v>
@@ -7208,7 +7196,7 @@
         <v>214</v>
       </c>
       <c r="C30" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D30" s="226">
         <v>1332.8432</v>
@@ -7226,7 +7214,7 @@
         <v>214</v>
       </c>
       <c r="C31" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D31" s="226">
         <v>516.88149999999996</v>
@@ -7244,7 +7232,7 @@
         <v>214</v>
       </c>
       <c r="C32" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D32" s="226">
         <v>1186.6908000000001</v>
@@ -7262,7 +7250,7 @@
         <v>214</v>
       </c>
       <c r="C33" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D33" s="226">
         <v>2091.6387</v>
@@ -7280,7 +7268,7 @@
         <v>214</v>
       </c>
       <c r="C34" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D34" s="226">
         <v>5208.4462000000003</v>
@@ -7298,7 +7286,7 @@
         <v>214</v>
       </c>
       <c r="C35" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D35" s="226">
         <v>1631.9170999999999</v>
@@ -7316,7 +7304,7 @@
         <v>214</v>
       </c>
       <c r="C36" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D36" s="226">
         <v>6871.9678000000004</v>
@@ -7334,7 +7322,7 @@
         <v>214</v>
       </c>
       <c r="C37" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D37" s="226">
         <v>4820.8257000000003</v>
@@ -7352,7 +7340,7 @@
         <v>214</v>
       </c>
       <c r="C38" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D38" s="226">
         <v>0</v>
@@ -7370,7 +7358,7 @@
         <v>214</v>
       </c>
       <c r="C39" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D39" s="226">
         <v>0</v>
@@ -7388,7 +7376,7 @@
         <v>214</v>
       </c>
       <c r="C40" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D40" s="226">
         <v>0</v>
@@ -7406,7 +7394,7 @@
         <v>214</v>
       </c>
       <c r="C41" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D41" s="226">
         <v>60.378300000000003</v>
@@ -7424,7 +7412,7 @@
         <v>214</v>
       </c>
       <c r="C42" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D42" s="226">
         <v>7267.0291999999999</v>
@@ -7442,7 +7430,7 @@
         <v>214</v>
       </c>
       <c r="C43" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D43" s="226">
         <v>9457.3282999999992</v>
@@ -7469,10 +7457,10 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="199" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C45" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D45" s="227">
         <v>864930.90700000001</v>
@@ -7499,18 +7487,18 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="199" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C47" s="200" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D47" s="226"/>
       <c r="E47" s="201"/>
       <c r="F47" s="214" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G47" s="214" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H47" s="233"/>
       <c r="I47" s="233"/>
@@ -7519,18 +7507,18 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="199" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C48" s="200" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D48" s="226"/>
       <c r="E48" s="201"/>
       <c r="F48" s="214" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G48" s="214" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H48" s="233"/>
       <c r="I48" s="233"/>
@@ -7539,20 +7527,20 @@
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="199" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C49" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D49" s="226">
         <v>628508.89240000001</v>
       </c>
       <c r="E49" s="201"/>
       <c r="F49" s="214" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G49" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H49" s="233">
         <v>639366.25690000004</v>
@@ -7569,20 +7557,20 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C50" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D50" s="226">
         <v>0</v>
       </c>
       <c r="E50" s="201"/>
       <c r="F50" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G50" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H50" s="233">
         <v>3355.8359</v>
@@ -7593,20 +7581,20 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C51" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D51" s="226">
         <v>0</v>
       </c>
       <c r="E51" s="201"/>
       <c r="F51" s="214" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G51" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H51" s="233">
         <v>26519.6548</v>
@@ -7623,20 +7611,20 @@
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C52" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D52" s="226">
         <v>30344.652300000002</v>
       </c>
       <c r="E52" s="201"/>
       <c r="F52" s="214" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G52" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H52" s="233">
         <v>31881.773799999999</v>
@@ -7653,20 +7641,20 @@
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="199" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C53" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D53" s="226">
         <v>3355.8359</v>
       </c>
       <c r="E53" s="201"/>
       <c r="F53" s="214" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G53" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H53" s="233">
         <v>75084.667499999996</v>
@@ -7683,10 +7671,10 @@
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C54" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D54" s="226">
         <v>21057.396499999999</v>
@@ -7696,7 +7684,7 @@
         <v>214</v>
       </c>
       <c r="G54" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H54" s="233">
         <v>83056.463099999994</v>
@@ -7713,20 +7701,20 @@
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C55" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D55" s="226">
         <v>969.43079999999998</v>
       </c>
       <c r="E55" s="201"/>
       <c r="F55" s="214" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G55" s="214" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H55" s="233">
         <v>0</v>
@@ -7737,10 +7725,10 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C56" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="226">
         <v>4491.2438000000002</v>
@@ -7755,20 +7743,20 @@
     </row>
     <row r="57" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C57" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D57" s="226">
         <v>31860.243399999999</v>
       </c>
       <c r="E57" s="201"/>
       <c r="F57" s="215" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G57" s="215" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H57" s="235">
         <v>859264.652</v>
@@ -7785,10 +7773,10 @@
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C58" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D58" s="226">
         <v>0</v>
@@ -7802,33 +7790,33 @@
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C59" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D59" s="226">
         <v>0</v>
       </c>
       <c r="E59" s="201"/>
       <c r="F59" s="214" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G59" s="214" t="s">
         <v>72</v>
       </c>
       <c r="H59" s="233" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I59" s="233"/>
       <c r="J59" s="219"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C60" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D60" s="226">
         <v>0</v>
@@ -7842,33 +7830,33 @@
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="199" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C61" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D61" s="226">
         <v>0</v>
       </c>
       <c r="E61" s="201"/>
       <c r="F61" s="214" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G61" s="214" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H61" s="233" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I61" s="233"/>
       <c r="J61" s="219"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="199" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C62" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D62" s="226">
         <v>75077.154500000004</v>
@@ -7885,7 +7873,7 @@
         <v>214</v>
       </c>
       <c r="C63" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D63" s="226">
         <v>3471.5511000000001</v>
@@ -7902,7 +7890,7 @@
         <v>214</v>
       </c>
       <c r="C64" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D64" s="226">
         <v>800.52049999999997</v>
@@ -7919,7 +7907,7 @@
         <v>214</v>
       </c>
       <c r="C65" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D65" s="226">
         <v>2378.2730999999999</v>
@@ -7936,7 +7924,7 @@
         <v>214</v>
       </c>
       <c r="C66" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D66" s="226">
         <v>5032.6646000000001</v>
@@ -7953,7 +7941,7 @@
         <v>214</v>
       </c>
       <c r="C67" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D67" s="226">
         <v>2443.7285999999999</v>
@@ -7970,7 +7958,7 @@
         <v>214</v>
       </c>
       <c r="C68" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D68" s="226">
         <v>2738.4059999999999</v>
@@ -7987,7 +7975,7 @@
         <v>214</v>
       </c>
       <c r="C69" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D69" s="226">
         <v>1244.4766999999999</v>
@@ -8004,7 +7992,7 @@
         <v>214</v>
       </c>
       <c r="C70" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D70" s="226">
         <v>1689.0364</v>
@@ -8021,7 +8009,7 @@
         <v>214</v>
       </c>
       <c r="C71" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D71" s="226">
         <v>4631.8999000000003</v>
@@ -8038,7 +8026,7 @@
         <v>214</v>
       </c>
       <c r="C72" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D72" s="226">
         <v>2115.9992999999999</v>
@@ -8055,7 +8043,7 @@
         <v>214</v>
       </c>
       <c r="C73" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D73" s="226">
         <v>3695.4479999999999</v>
@@ -8072,7 +8060,7 @@
         <v>214</v>
       </c>
       <c r="C74" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D74" s="226">
         <v>3832.8202999999999</v>
@@ -8089,7 +8077,7 @@
         <v>214</v>
       </c>
       <c r="C75" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D75" s="226">
         <v>6525.9380000000001</v>
@@ -8106,7 +8094,7 @@
         <v>214</v>
       </c>
       <c r="C76" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D76" s="226">
         <v>0</v>
@@ -8123,7 +8111,7 @@
         <v>214</v>
       </c>
       <c r="C77" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D77" s="226">
         <v>0</v>
@@ -8140,7 +8128,7 @@
         <v>214</v>
       </c>
       <c r="C78" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D78" s="226">
         <v>0</v>
@@ -8157,7 +8145,7 @@
         <v>214</v>
       </c>
       <c r="C79" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D79" s="226">
         <v>52.5762</v>
@@ -8174,7 +8162,7 @@
         <v>214</v>
       </c>
       <c r="C80" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D80" s="226">
         <v>23411.458500000001</v>
@@ -8191,7 +8179,7 @@
         <v>214</v>
       </c>
       <c r="C81" s="200" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D81" s="226">
         <v>5345.1895999999997</v>
@@ -8216,10 +8204,10 @@
     </row>
     <row r="83" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="202" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C83" s="203" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D83" s="229">
         <v>865074.83640000003</v>
@@ -8657,7 +8645,7 @@
     </row>
     <row r="2" spans="1:20" s="121" customFormat="1" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B2" s="109" t="s">
         <v>87</v>
@@ -8749,7 +8737,7 @@
         <v>3</v>
       </c>
       <c r="O3" s="127" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P3" s="127"/>
     </row>
@@ -10328,7 +10316,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -10340,7 +10328,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="245" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D3" s="246" t="s">
         <v>127</v>
@@ -10351,10 +10339,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="173" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C4" s="173" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D4" s="240"/>
     </row>
@@ -10363,10 +10351,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="173" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C5" s="173" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D5" s="240"/>
     </row>
@@ -10375,10 +10363,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="173" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C6" s="173" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D6" s="240"/>
     </row>
@@ -10387,10 +10375,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="173" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="173" t="s">
         <v>298</v>
-      </c>
-      <c r="C7" s="173" t="s">
-        <v>300</v>
       </c>
       <c r="D7" s="240"/>
     </row>
@@ -10402,10 +10390,10 @@
         <v>177</v>
       </c>
       <c r="C8" s="173" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" s="240" t="s">
         <v>301</v>
-      </c>
-      <c r="D8" s="240" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -10416,10 +10404,10 @@
         <v>178</v>
       </c>
       <c r="C9" s="247" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D9" s="240" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -10430,10 +10418,10 @@
         <v>179</v>
       </c>
       <c r="C10" s="247" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D10" s="240" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -10444,10 +10432,10 @@
         <v>180</v>
       </c>
       <c r="C11" s="247" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D11" s="240" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -10458,10 +10446,10 @@
         <v>181</v>
       </c>
       <c r="C12" s="247" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D12" s="240" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -10472,10 +10460,10 @@
         <v>182</v>
       </c>
       <c r="C13" s="247" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D13" s="240" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -10486,10 +10474,10 @@
         <v>183</v>
       </c>
       <c r="C14" s="247" t="s">
+        <v>304</v>
+      </c>
+      <c r="D14" s="240" t="s">
         <v>306</v>
-      </c>
-      <c r="D14" s="240" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -10500,7 +10488,7 @@
         <v>184</v>
       </c>
       <c r="C15" s="247" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D15" s="240"/>
     </row>
@@ -10512,7 +10500,7 @@
         <v>185</v>
       </c>
       <c r="C16" s="247" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D16" s="240"/>
     </row>
@@ -10524,7 +10512,7 @@
         <v>186</v>
       </c>
       <c r="C17" s="248" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D17" s="243"/>
     </row>
@@ -10539,74 +10527,112 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="9.140625" style="249"/>
-    <col min="16" max="16" width="37.140625" style="249" customWidth="1"/>
-    <col min="17" max="17" width="76.5703125" style="144" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="249"/>
+    <col min="1" max="1" width="5.7109375" style="249" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="249" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="249" customWidth="1"/>
+    <col min="4" max="4" width="76.5703125" style="144" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="249"/>
+    <col min="7" max="7" width="10.85546875" style="249" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="249"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="249">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="265"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="266" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" s="267"/>
+      <c r="F1" s="249" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="268" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2" s="269" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" s="269" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="144" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" s="144" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="250">
+        <v>1</v>
+      </c>
+      <c r="B3" s="250"/>
+      <c r="C3" s="250" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" s="251" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" s="249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="250">
         <v>2</v>
       </c>
-      <c r="B1" s="249" t="s">
-        <v>237</v>
-      </c>
-      <c r="O1" s="250" t="s">
+      <c r="B4" s="250"/>
+      <c r="C4" s="250" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="251" t="s">
         <v>311</v>
       </c>
-      <c r="P1" s="250" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="249">
+        <v>3</v>
+      </c>
+      <c r="B5" s="249">
+        <v>1</v>
+      </c>
+      <c r="C5" s="249" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="Q1" s="251" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="O2" s="250">
-        <v>1</v>
-      </c>
-      <c r="P2" s="250" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q2" s="251" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="249">
-        <v>3</v>
-      </c>
-      <c r="B3" s="249" t="s">
-        <v>238</v>
-      </c>
-      <c r="O3" s="250">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="249">
+        <v>4</v>
+      </c>
+      <c r="B6" s="249">
         <v>2</v>
       </c>
-      <c r="P3" s="250" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q3" s="251" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O4" s="249">
-        <v>3</v>
-      </c>
-      <c r="P4" s="249" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q4" s="144" t="s">
-        <v>317</v>
+      <c r="C6" s="249" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="144" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="249">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Routine: Still debugging NBr32 ipython
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB2663B3-CF85-4E29-B74B-672DB375EEE7}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487BE5E9-D371-4845-BEDA-A29752381511}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -594,6 +594,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E42EC14D-BD5A-400D-A934-346EA61A0CA2}</author>
+    <author>tc={928E89C2-6353-4AC6-8BD4-DDDAB50745FF}</author>
   </authors>
   <commentList>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
@@ -602,6 +603,14 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Check source code for more.</t>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{928E89C2-6353-4AC6-8BD4-DDDAB50745FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not important in my case as I go for full transient.</t>
       </text>
     </comment>
   </commentList>
@@ -664,7 +673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="325">
   <si>
     <t>#</t>
   </si>
@@ -2375,6 +2384,18 @@
   </si>
   <si>
     <t>Chech screenshot</t>
+  </si>
+  <si>
+    <t>PRJ file with SS block(s) causes an error.</t>
+  </si>
+  <si>
+    <t>imod.open_projectfile_data + SS</t>
+  </si>
+  <si>
+    <t>mf6.Modflow6Simulation + winter/summer</t>
+  </si>
+  <si>
+    <t>winter/summer can be loaded from PRJ, but when you try to make a sim</t>
   </si>
 </sst>
 </file>
@@ -3854,6 +3875,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3891,21 +3927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4640,6 +4661,9 @@
   <threadedComment ref="D3" dT="2025-07-15T09:17:30.76" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{E42EC14D-BD5A-400D-A934-346EA61A0CA2}">
     <text>Check source code for more.</text>
   </threadedComment>
+  <threadedComment ref="D7" dT="2025-07-25T10:06:37.84" personId="{03CB0575-C3E6-4F90-B161-647A816C1753}" id="{928E89C2-6353-4AC6-8BD4-DDDAB50745FF}">
+    <text>Not important in my case as I go for full transient.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -5128,21 +5152,21 @@
       <c r="O11" s="181"/>
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="253" t="s">
+      <c r="E13" s="258" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="253"/>
-      <c r="G13" s="253"/>
-      <c r="H13" s="253"/>
-      <c r="I13" s="253"/>
-      <c r="J13" s="253"/>
+      <c r="F13" s="258"/>
+      <c r="G13" s="258"/>
+      <c r="H13" s="258"/>
+      <c r="I13" s="258"/>
+      <c r="J13" s="258"/>
       <c r="K13" s="194"/>
-      <c r="L13" s="252" t="s">
+      <c r="L13" s="257" t="s">
         <v>256</v>
       </c>
-      <c r="M13" s="252"/>
-      <c r="N13" s="252"/>
-      <c r="O13" s="252"/>
+      <c r="M13" s="257"/>
+      <c r="N13" s="257"/>
+      <c r="O13" s="257"/>
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">
@@ -5322,50 +5346,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="260" t="s">
+      <c r="B6" s="265" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
+      <c r="C6" s="266"/>
+      <c r="D6" s="266"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="262" t="s">
+      <c r="F6" s="267" t="s">
         <v>285</v>
       </c>
-      <c r="G6" s="262"/>
-      <c r="H6" s="262"/>
-      <c r="I6" s="262"/>
-      <c r="J6" s="262"/>
+      <c r="G6" s="267"/>
+      <c r="H6" s="267"/>
+      <c r="I6" s="267"/>
+      <c r="J6" s="267"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="258" t="s">
+      <c r="B7" s="263" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="259"/>
-      <c r="D7" s="259"/>
+      <c r="C7" s="264"/>
+      <c r="D7" s="264"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="257" t="s">
+      <c r="F7" s="262" t="s">
         <v>272</v>
       </c>
-      <c r="G7" s="257"/>
-      <c r="H7" s="257"/>
-      <c r="I7" s="257"/>
-      <c r="J7" s="257"/>
+      <c r="G7" s="262"/>
+      <c r="H7" s="262"/>
+      <c r="I7" s="262"/>
+      <c r="J7" s="262"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="254" t="s">
+      <c r="B8" s="259" t="s">
         <v>288</v>
       </c>
-      <c r="C8" s="255"/>
+      <c r="C8" s="260"/>
       <c r="D8" s="225" t="s">
         <v>275</v>
       </c>
       <c r="E8" s="210"/>
-      <c r="F8" s="256" t="s">
+      <c r="F8" s="261" t="s">
         <v>288</v>
       </c>
-      <c r="G8" s="256"/>
+      <c r="G8" s="261"/>
       <c r="H8" s="232" t="s">
         <v>275</v>
       </c>
@@ -6680,50 +6704,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="260" t="s">
+      <c r="B6" s="265" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
+      <c r="C6" s="266"/>
+      <c r="D6" s="266"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="262" t="s">
+      <c r="F6" s="267" t="s">
         <v>285</v>
       </c>
-      <c r="G6" s="262"/>
-      <c r="H6" s="262"/>
-      <c r="I6" s="262"/>
-      <c r="J6" s="262"/>
+      <c r="G6" s="267"/>
+      <c r="H6" s="267"/>
+      <c r="I6" s="267"/>
+      <c r="J6" s="267"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="258" t="s">
+      <c r="B7" s="263" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="259"/>
-      <c r="D7" s="259"/>
+      <c r="C7" s="264"/>
+      <c r="D7" s="264"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="257" t="s">
+      <c r="F7" s="262" t="s">
         <v>272</v>
       </c>
-      <c r="G7" s="257"/>
-      <c r="H7" s="257"/>
-      <c r="I7" s="257"/>
-      <c r="J7" s="257"/>
+      <c r="G7" s="262"/>
+      <c r="H7" s="262"/>
+      <c r="I7" s="262"/>
+      <c r="J7" s="262"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="268" t="s">
         <v>288</v>
       </c>
-      <c r="C8" s="264"/>
+      <c r="C8" s="269"/>
       <c r="D8" s="236" t="s">
         <v>275</v>
       </c>
       <c r="E8" s="209"/>
-      <c r="F8" s="256" t="s">
+      <c r="F8" s="261" t="s">
         <v>288</v>
       </c>
-      <c r="G8" s="256"/>
+      <c r="G8" s="261"/>
       <c r="H8" s="232" t="s">
         <v>275</v>
       </c>
@@ -10530,7 +10554,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10545,27 +10569,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="265"/>
-      <c r="B1" s="265"/>
-      <c r="C1" s="266" t="s">
+      <c r="A1" s="252"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="253" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="267"/>
+      <c r="D1" s="254"/>
       <c r="F1" s="249" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="268" t="s">
+      <c r="A2" s="255" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="268" t="s">
+      <c r="B2" s="255" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="256" t="s">
         <v>313</v>
       </c>
-      <c r="D2" s="269" t="s">
+      <c r="D2" s="256" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="144" t="s">
@@ -10628,6 +10652,28 @@
       </c>
       <c r="D6" s="144" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="249">
+        <v>5</v>
+      </c>
+      <c r="C7" s="249" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" s="144" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="249">
+        <v>6</v>
+      </c>
+      <c r="C8" s="249" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" s="144" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
imod-python: everything's loaded, but write fails
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487BE5E9-D371-4845-BEDA-A29752381511}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD468723-9E1D-4CAD-8C51-915E295B2648}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -673,7 +673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294966614" uniqueCount="326">
   <si>
     <t>#</t>
   </si>
@@ -2396,6 +2396,9 @@
   </si>
   <si>
     <t>winter/summer can be loaded from PRJ, but when you try to make a sim</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -3183,7 +3186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3927,6 +3930,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10554,7 +10560,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10676,6 +10682,14 @@
         <v>324</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="144"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="270" t="s">
+        <v>325</v>
+      </c>
+    </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28" s="249">
         <v>2</v>

</xml_diff>

<commit_message>
Cleanup before other edits
Acronyms.xlsx moved from Thesis repo to WS_Mdl, so that it's public.
imod_python_init_NBr32.ipynb edited (slight clean-up. Nothing major)
open_ commands touched by ruff (separates remote from local imports)
setup.py: added some required libs, so that they get installed with pixi
pixi attempt at running imod_python_init_NBr32.ipynb
</commit_message>
<xml_diff>
--- a/Mng/WS_Mdl_Ipvs.xlsx
+++ b/Mng/WS_Mdl_Ipvs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/m_karampasis_uu_nl/Documents/WS_Mdl/Mng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD468723-9E1D-4CAD-8C51-915E295B2648}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{5E3970D3-2CD9-4A5D-9889-3973511BE780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CD5AB8F-5ABF-413C-B675-B1B083E63F2F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,7 +673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294966614" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="328">
   <si>
     <t>#</t>
   </si>
@@ -2399,6 +2399,16 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Sim_MF6 = mf6.Modflow6Simulation.from_imod5_data(PRJ_regrid, period_data, times)</t>
+  </si>
+  <si>
+    <t>Gives Keyerror: 0. This is related to a WEL file of my PRJ file.
+I've found a fix - need to insert:
+    well_rate = well_rate.reset_index(drop=True)
+before     intermediate_df = pd.merge(... 
+C:\mamba_envs\WS\Lib\site-packages\imod\util\expnd_repetitions.py</t>
   </si>
 </sst>
 </file>
@@ -3892,6 +3902,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3930,9 +3943,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4076,7 +4086,7 @@
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>45314</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>151528</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4102,6 +4112,50 @@
         <a:xfrm>
           <a:off x="9744075" y="588920"/>
           <a:ext cx="13532714" cy="5106158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>256214</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>113833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F42142CE-4C03-7E97-A1C8-95F0383EA022}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9705975" y="13354050"/>
+          <a:ext cx="7685714" cy="3733333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5158,21 +5212,21 @@
       <c r="O11" s="181"/>
     </row>
     <row r="13" spans="1:15" s="193" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="258" t="s">
+      <c r="E13" s="259" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="258"/>
-      <c r="G13" s="258"/>
-      <c r="H13" s="258"/>
-      <c r="I13" s="258"/>
-      <c r="J13" s="258"/>
+      <c r="F13" s="259"/>
+      <c r="G13" s="259"/>
+      <c r="H13" s="259"/>
+      <c r="I13" s="259"/>
+      <c r="J13" s="259"/>
       <c r="K13" s="194"/>
-      <c r="L13" s="257" t="s">
+      <c r="L13" s="258" t="s">
         <v>256</v>
       </c>
-      <c r="M13" s="257"/>
-      <c r="N13" s="257"/>
-      <c r="O13" s="257"/>
+      <c r="M13" s="258"/>
+      <c r="N13" s="258"/>
+      <c r="O13" s="258"/>
     </row>
     <row r="14" spans="1:15" s="145" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="175" t="s">
@@ -5352,50 +5406,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="265" t="s">
+      <c r="B6" s="266" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="266"/>
-      <c r="D6" s="266"/>
+      <c r="C6" s="267"/>
+      <c r="D6" s="267"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="267" t="s">
+      <c r="F6" s="268" t="s">
         <v>285</v>
       </c>
-      <c r="G6" s="267"/>
-      <c r="H6" s="267"/>
-      <c r="I6" s="267"/>
-      <c r="J6" s="267"/>
+      <c r="G6" s="268"/>
+      <c r="H6" s="268"/>
+      <c r="I6" s="268"/>
+      <c r="J6" s="268"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="263" t="s">
+      <c r="B7" s="264" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="264"/>
-      <c r="D7" s="264"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="265"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="262" t="s">
+      <c r="F7" s="263" t="s">
         <v>272</v>
       </c>
-      <c r="G7" s="262"/>
-      <c r="H7" s="262"/>
-      <c r="I7" s="262"/>
-      <c r="J7" s="262"/>
+      <c r="G7" s="263"/>
+      <c r="H7" s="263"/>
+      <c r="I7" s="263"/>
+      <c r="J7" s="263"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="259" t="s">
+      <c r="B8" s="260" t="s">
         <v>288</v>
       </c>
-      <c r="C8" s="260"/>
+      <c r="C8" s="261"/>
       <c r="D8" s="225" t="s">
         <v>275</v>
       </c>
       <c r="E8" s="210"/>
-      <c r="F8" s="261" t="s">
+      <c r="F8" s="262" t="s">
         <v>288</v>
       </c>
-      <c r="G8" s="261"/>
+      <c r="G8" s="262"/>
       <c r="H8" s="232" t="s">
         <v>275</v>
       </c>
@@ -6710,50 +6764,50 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="265" t="s">
+      <c r="B6" s="266" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="266"/>
-      <c r="D6" s="266"/>
+      <c r="C6" s="267"/>
+      <c r="D6" s="267"/>
       <c r="E6" s="211"/>
-      <c r="F6" s="267" t="s">
+      <c r="F6" s="268" t="s">
         <v>285</v>
       </c>
-      <c r="G6" s="267"/>
-      <c r="H6" s="267"/>
-      <c r="I6" s="267"/>
-      <c r="J6" s="267"/>
+      <c r="G6" s="268"/>
+      <c r="H6" s="268"/>
+      <c r="I6" s="268"/>
+      <c r="J6" s="268"/>
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="263" t="s">
+      <c r="B7" s="264" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="264"/>
-      <c r="D7" s="264"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="265"/>
       <c r="E7" s="209"/>
-      <c r="F7" s="262" t="s">
+      <c r="F7" s="263" t="s">
         <v>272</v>
       </c>
-      <c r="G7" s="262"/>
-      <c r="H7" s="262"/>
-      <c r="I7" s="262"/>
-      <c r="J7" s="262"/>
+      <c r="G7" s="263"/>
+      <c r="H7" s="263"/>
+      <c r="I7" s="263"/>
+      <c r="J7" s="263"/>
       <c r="K7" s="201"/>
     </row>
     <row r="8" spans="1:11" s="144" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="268" t="s">
+      <c r="B8" s="269" t="s">
         <v>288</v>
       </c>
-      <c r="C8" s="269"/>
+      <c r="C8" s="270"/>
       <c r="D8" s="236" t="s">
         <v>275</v>
       </c>
       <c r="E8" s="209"/>
-      <c r="F8" s="261" t="s">
+      <c r="F8" s="262" t="s">
         <v>288</v>
       </c>
-      <c r="G8" s="261"/>
+      <c r="G8" s="262"/>
       <c r="H8" s="232" t="s">
         <v>275</v>
       </c>
@@ -10557,10 +10611,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10682,17 +10736,30 @@
         <v>324</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="144"/>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="249">
+        <v>7</v>
+      </c>
+      <c r="C9" s="144" t="s">
+        <v>326</v>
+      </c>
+      <c r="D9" s="144" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="270" t="s">
+      <c r="C10" s="257" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28" s="249">
         <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="249">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>